<commit_message>
Error Tracker window is now working perfectly.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -32,7 +32,7 @@
     <numFmt numFmtId="167" formatCode="d\-mmm\-yy"/>
     <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -103,6 +103,11 @@
       <family val="2"/>
       <b val="1"/>
       <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -581,7 +586,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="232">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -1219,6 +1224,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2690,9 +2704,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="H19:Q19"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="F5:H5"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -8472,7 +8486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
@@ -8645,22 +8659,44 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="104" t="inlineStr">
         <is>
           <t>pe</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="104" t="inlineStr">
         <is>
           <t>rs</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="104" t="inlineStr">
         <is>
           <t>on</t>
         </is>
       </c>
       <c r="D9" s="231" t="inlineStr">
+        <is>
+          <t>22-Jun-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="104" t="inlineStr">
+        <is>
+          <t>bv</t>
+        </is>
+      </c>
+      <c r="B10" s="104" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="C10" s="104" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="D10" s="231" t="inlineStr">
         <is>
           <t>22-Jun-2024</t>
         </is>
@@ -8679,7 +8715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
@@ -8958,6 +8994,134 @@
       <c r="D19" s="215" t="n"/>
       <c r="E19" s="216" t="n"/>
       <c r="F19" s="216" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="231" t="inlineStr">
+        <is>
+          <t>22-Jun-2024</t>
+        </is>
+      </c>
+      <c r="B20" s="104" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C20" s="104" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="D20" s="104" t="inlineStr">
+        <is>
+          <t>sadf</t>
+        </is>
+      </c>
+      <c r="E20" s="104" t="inlineStr">
+        <is>
+          <t>sadf</t>
+        </is>
+      </c>
+      <c r="F20" s="104" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="231" t="inlineStr">
+        <is>
+          <t>22-Jun-2024</t>
+        </is>
+      </c>
+      <c r="B21" s="104" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C21" s="104" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D21" s="104" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E21" s="104" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="F21" s="104" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="232" t="inlineStr">
+        <is>
+          <t>22-Jun-2024</t>
+        </is>
+      </c>
+      <c r="B22" s="233" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C22" s="233" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D22" s="233" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E22" s="234" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F22" s="234" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="231" t="inlineStr">
+        <is>
+          <t>22-Jun-2024</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>gsdfdf</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>fdgs</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>sdfg</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>sdfg</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
Completed Truck Fill % entry
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -10219,10 +10219,8 @@
       <c r="FO13" s="199" t="n">
         <v>0.9</v>
       </c>
-      <c r="FP13" s="199" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="FP13" s="199" t="n">
+        <v>0.9615384615384616</v>
       </c>
       <c r="FQ13" s="199" t="inlineStr"/>
       <c r="FR13" s="199" t="inlineStr"/>

</xml_diff>

<commit_message>
Added an auto-load funtion after a file is selected the first time.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -1710,10 +1710,7 @@
       <c r="Q3" s="115" t="n"/>
     </row>
     <row r="4" ht="14.25" customHeight="1" s="106">
-      <c r="B4" s="116">
-        <f>TODAY()</f>
-        <v/>
-      </c>
+      <c r="B4" s="116" t="inlineStr"/>
       <c r="D4" s="117" t="inlineStr">
         <is>
           <t>Days Without Incident</t>
@@ -2687,9 +2684,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="H19:Q19"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="F5:H5"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -2913,7 +2910,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -4652,7 +4649,7 @@
           <t>Haz ID's</t>
         </is>
       </c>
-      <c r="C3" s="104" t="n"/>
+      <c r="C3" s="104" t="inlineStr"/>
       <c r="D3" s="104" t="n"/>
       <c r="E3" s="104" t="n"/>
       <c r="F3" s="104" t="n"/>
@@ -5212,7 +5209,7 @@
           <t>Safety Gemba Walk</t>
         </is>
       </c>
-      <c r="C4" s="104" t="n"/>
+      <c r="C4" s="104" t="inlineStr"/>
       <c r="D4" s="104" t="n"/>
       <c r="E4" s="104" t="n"/>
       <c r="F4" s="104" t="n"/>
@@ -5768,7 +5765,7 @@
           <t>7S (Zone 26)</t>
         </is>
       </c>
-      <c r="C5" s="104" t="n"/>
+      <c r="C5" s="104" t="inlineStr"/>
       <c r="D5" s="104" t="n"/>
       <c r="E5" s="104" t="n"/>
       <c r="F5" s="104" t="n"/>
@@ -6302,7 +6299,7 @@
           <t>7S (Zone 51)</t>
         </is>
       </c>
-      <c r="C6" s="104" t="n"/>
+      <c r="C6" s="104" t="inlineStr"/>
       <c r="D6" s="104" t="n"/>
       <c r="E6" s="104" t="n"/>
       <c r="F6" s="104" t="n"/>
@@ -12493,7 +12490,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -12526,17 +12523,22 @@
     <row r="2" ht="15" customHeight="1" s="106">
       <c r="A2" s="104" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" s="104" t="inlineStr">
         <is>
-          <t>Nyman</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" s="104" t="inlineStr">
         <is>
-          <t>Helping to keep both areas clean and organized</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2" s="104" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -12656,7 +12658,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -12901,7 +12903,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14602,7 +14604,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
Modifying the recomendations window and fixing the iverlapping saving methods.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -2910,7 +2910,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -12490,7 +12490,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -12521,26 +12521,10 @@
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="106">
-      <c r="A2" s="104" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" s="104" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" s="104" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D2" s="104" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="A2" s="104" t="inlineStr"/>
+      <c r="B2" s="104" t="inlineStr"/>
+      <c r="C2" s="104" t="inlineStr"/>
+      <c r="D2" s="104" t="inlineStr"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="106">
       <c r="A3" s="104" t="inlineStr">
@@ -12658,7 +12642,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -12903,7 +12887,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14604,7 +14588,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
Got the recognition entry sheet working correctly.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -1710,7 +1710,11 @@
       <c r="Q3" s="115" t="n"/>
     </row>
     <row r="4" ht="14.25" customHeight="1" s="106">
-      <c r="B4" s="116" t="inlineStr"/>
+      <c r="B4" s="116" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
       <c r="D4" s="117" t="inlineStr">
         <is>
           <t>Days Without Incident</t>
@@ -2684,9 +2688,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="H19:Q19"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="H19:Q19"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -2910,7 +2914,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -4649,7 +4653,11 @@
           <t>Haz ID's</t>
         </is>
       </c>
-      <c r="C3" s="104" t="inlineStr"/>
+      <c r="C3" s="104" t="inlineStr">
+        <is>
+          <t>yygi</t>
+        </is>
+      </c>
       <c r="D3" s="104" t="n"/>
       <c r="E3" s="104" t="n"/>
       <c r="F3" s="104" t="n"/>
@@ -5209,7 +5217,11 @@
           <t>Safety Gemba Walk</t>
         </is>
       </c>
-      <c r="C4" s="104" t="inlineStr"/>
+      <c r="C4" s="104" t="inlineStr">
+        <is>
+          <t>iu</t>
+        </is>
+      </c>
       <c r="D4" s="104" t="n"/>
       <c r="E4" s="104" t="n"/>
       <c r="F4" s="104" t="n"/>
@@ -5765,7 +5777,11 @@
           <t>7S (Zone 26)</t>
         </is>
       </c>
-      <c r="C5" s="104" t="inlineStr"/>
+      <c r="C5" s="104" t="inlineStr">
+        <is>
+          <t>iug</t>
+        </is>
+      </c>
       <c r="D5" s="104" t="n"/>
       <c r="E5" s="104" t="n"/>
       <c r="F5" s="104" t="n"/>
@@ -6299,7 +6315,11 @@
           <t>7S (Zone 51)</t>
         </is>
       </c>
-      <c r="C6" s="104" t="inlineStr"/>
+      <c r="C6" s="104" t="inlineStr">
+        <is>
+          <t>iug</t>
+        </is>
+      </c>
       <c r="D6" s="104" t="n"/>
       <c r="E6" s="104" t="n"/>
       <c r="F6" s="104" t="n"/>
@@ -12484,13 +12504,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -12521,10 +12541,26 @@
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="106">
-      <c r="A2" s="104" t="inlineStr"/>
-      <c r="B2" s="104" t="inlineStr"/>
-      <c r="C2" s="104" t="inlineStr"/>
-      <c r="D2" s="104" t="inlineStr"/>
+      <c r="A2" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="B2" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="C2" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="D2" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="106">
       <c r="A3" s="104" t="inlineStr">
@@ -12620,6 +12656,182 @@
       <c r="D7" s="210" t="inlineStr">
         <is>
           <t>21-May-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="B8" s="104" t="inlineStr">
+        <is>
+          <t>pee</t>
+        </is>
+      </c>
+      <c r="C8" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="D8" s="104" t="inlineStr">
+        <is>
+          <t>pee</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="B9" s="104" t="inlineStr">
+        <is>
+          <t>pee</t>
+        </is>
+      </c>
+      <c r="C9" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="D9" s="104" t="inlineStr">
+        <is>
+          <t>pee</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="B10" s="104" t="inlineStr">
+        <is>
+          <t>pee</t>
+        </is>
+      </c>
+      <c r="C10" s="104" t="inlineStr">
+        <is>
+          <t>poo</t>
+        </is>
+      </c>
+      <c r="D10" s="104" t="inlineStr">
+        <is>
+          <t>pee</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="B11" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="C11" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="D11" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="B12" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="C12" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="D12" s="104" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="104" t="inlineStr">
+        <is>
+          <t>popa</t>
+        </is>
+      </c>
+      <c r="B13" s="104" t="inlineStr">
+        <is>
+          <t>popa</t>
+        </is>
+      </c>
+      <c r="C13" s="104" t="inlineStr">
+        <is>
+          <t>popa</t>
+        </is>
+      </c>
+      <c r="D13" s="104" t="inlineStr">
+        <is>
+          <t>popa</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="104" t="inlineStr">
+        <is>
+          <t>papa</t>
+        </is>
+      </c>
+      <c r="B14" s="104" t="inlineStr">
+        <is>
+          <t>popo</t>
+        </is>
+      </c>
+      <c r="C14" s="104" t="inlineStr">
+        <is>
+          <t>pupu</t>
+        </is>
+      </c>
+      <c r="D14" s="104" t="inlineStr">
+        <is>
+          <t>pepe</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>oo</t>
         </is>
       </c>
     </row>
@@ -12642,7 +12854,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -12887,7 +13099,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14588,7 +14800,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
"Enter" now saves the data and resets the selected entry field to the top.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1710,11 +1710,7 @@
       <c r="Q3" s="115" t="n"/>
     </row>
     <row r="4" ht="14.25" customHeight="1" s="106">
-      <c r="B4" s="116" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
+      <c r="B4" s="116" t="inlineStr"/>
       <c r="D4" s="117" t="inlineStr">
         <is>
           <t>Days Without Incident</t>
@@ -4653,11 +4649,7 @@
           <t>Haz ID's</t>
         </is>
       </c>
-      <c r="C3" s="104" t="inlineStr">
-        <is>
-          <t>yygi</t>
-        </is>
-      </c>
+      <c r="C3" s="104" t="inlineStr"/>
       <c r="D3" s="104" t="n"/>
       <c r="E3" s="104" t="n"/>
       <c r="F3" s="104" t="n"/>
@@ -5217,11 +5209,7 @@
           <t>Safety Gemba Walk</t>
         </is>
       </c>
-      <c r="C4" s="104" t="inlineStr">
-        <is>
-          <t>iu</t>
-        </is>
-      </c>
+      <c r="C4" s="104" t="inlineStr"/>
       <c r="D4" s="104" t="n"/>
       <c r="E4" s="104" t="n"/>
       <c r="F4" s="104" t="n"/>
@@ -5777,11 +5765,7 @@
           <t>7S (Zone 26)</t>
         </is>
       </c>
-      <c r="C5" s="104" t="inlineStr">
-        <is>
-          <t>iug</t>
-        </is>
-      </c>
+      <c r="C5" s="104" t="inlineStr"/>
       <c r="D5" s="104" t="n"/>
       <c r="E5" s="104" t="n"/>
       <c r="F5" s="104" t="n"/>
@@ -6315,11 +6299,7 @@
           <t>7S (Zone 51)</t>
         </is>
       </c>
-      <c r="C6" s="104" t="inlineStr">
-        <is>
-          <t>iug</t>
-        </is>
-      </c>
+      <c r="C6" s="104" t="inlineStr"/>
       <c r="D6" s="104" t="n"/>
       <c r="E6" s="104" t="n"/>
       <c r="F6" s="104" t="n"/>
@@ -12504,7 +12484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
@@ -12814,24 +12794,90 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="104" t="inlineStr">
         <is>
           <t>oo</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="104" t="inlineStr">
         <is>
           <t>oo</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="104" t="inlineStr">
         <is>
           <t>oo</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="104" t="inlineStr">
         <is>
           <t>oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="B16" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="C16" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="D16" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="B17" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="C17" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="D17" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="B18" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="C18" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
+        </is>
+      </c>
+      <c r="D18" s="104" t="inlineStr">
+        <is>
+          <t>op</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a date entry above the data
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -2684,9 +2684,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="H19:Q19"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="F5:H5"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -2910,7 +2910,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -12484,13 +12484,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -12878,6 +12878,28 @@
       <c r="D18" s="104" t="inlineStr">
         <is>
           <t>op</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Fart</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>poopy</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Today</t>
         </is>
       </c>
     </row>
@@ -12900,7 +12922,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -13145,7 +13167,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14846,7 +14868,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
Added a toggle for "Days without Incident"
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -2684,9 +2684,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="H19:Q19"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="H19:Q19"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -2910,7 +2910,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -4604,8 +4604,16 @@
       <c r="LQ2" s="104" t="n"/>
       <c r="LR2" s="104" t="n"/>
       <c r="LS2" s="104" t="n"/>
-      <c r="LT2" s="104" t="n"/>
-      <c r="LU2" s="104" t="n"/>
+      <c r="LT2" s="104" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+      <c r="LU2" s="104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="LV2" s="104" t="n"/>
       <c r="LW2" s="104" t="n"/>
       <c r="LX2" s="104" t="n"/>
@@ -5164,8 +5172,12 @@
       <c r="LQ3" s="104" t="n"/>
       <c r="LR3" s="104" t="n"/>
       <c r="LS3" s="104" t="n"/>
-      <c r="LT3" s="104" t="n"/>
-      <c r="LU3" s="104" t="n"/>
+      <c r="LT3" s="104" t="inlineStr">
+        <is>
+          <t>oppo</t>
+        </is>
+      </c>
+      <c r="LU3" s="104" t="inlineStr"/>
       <c r="LV3" s="104" t="n"/>
       <c r="LW3" s="104" t="n"/>
       <c r="LX3" s="104" t="n"/>
@@ -5720,8 +5732,12 @@
       <c r="LQ4" s="104" t="n"/>
       <c r="LR4" s="104" t="n"/>
       <c r="LS4" s="104" t="n"/>
-      <c r="LT4" s="104" t="n"/>
-      <c r="LU4" s="104" t="n"/>
+      <c r="LT4" s="104" t="inlineStr">
+        <is>
+          <t>popo</t>
+        </is>
+      </c>
+      <c r="LU4" s="104" t="inlineStr"/>
       <c r="LV4" s="104" t="n"/>
       <c r="LW4" s="104" t="n"/>
       <c r="LX4" s="104" t="n"/>
@@ -6254,8 +6270,12 @@
       <c r="LQ5" s="104" t="n"/>
       <c r="LR5" s="104" t="n"/>
       <c r="LS5" s="104" t="n"/>
-      <c r="LT5" s="104" t="n"/>
-      <c r="LU5" s="104" t="n"/>
+      <c r="LT5" s="104" t="inlineStr">
+        <is>
+          <t>opop</t>
+        </is>
+      </c>
+      <c r="LU5" s="104" t="inlineStr"/>
       <c r="LV5" s="104" t="n"/>
       <c r="LW5" s="104" t="n"/>
       <c r="LX5" s="104" t="n"/>
@@ -6782,8 +6802,12 @@
       <c r="LQ6" s="104" t="n"/>
       <c r="LR6" s="104" t="n"/>
       <c r="LS6" s="104" t="n"/>
-      <c r="LT6" s="104" t="n"/>
-      <c r="LU6" s="104" t="n"/>
+      <c r="LT6" s="104" t="inlineStr">
+        <is>
+          <t>ooop</t>
+        </is>
+      </c>
+      <c r="LU6" s="104" t="inlineStr"/>
       <c r="LV6" s="104" t="n"/>
       <c r="LW6" s="104" t="n"/>
       <c r="LX6" s="104" t="n"/>
@@ -7135,6 +7159,7 @@
           <t>bii</t>
         </is>
       </c>
+      <c r="LU7" s="104" t="inlineStr"/>
     </row>
     <row r="8" ht="15" customHeight="1" s="106">
       <c r="A8" s="104" t="n"/>
@@ -7665,7 +7690,7 @@
       <c r="LR8" s="104" t="n"/>
       <c r="LS8" s="104" t="n"/>
       <c r="LT8" s="104" t="n"/>
-      <c r="LU8" s="104" t="n"/>
+      <c r="LU8" s="104" t="inlineStr"/>
       <c r="LV8" s="104" t="n"/>
       <c r="LW8" s="104" t="n"/>
       <c r="LX8" s="104" t="n"/>
@@ -7819,6 +7844,7 @@
           <t>h</t>
         </is>
       </c>
+      <c r="LU9" s="104" t="inlineStr"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="106">
       <c r="A10" s="199" t="n"/>
@@ -8215,7 +8241,7 @@
       <c r="LR10" s="199" t="n"/>
       <c r="LS10" s="199" t="n"/>
       <c r="LT10" s="199" t="n"/>
-      <c r="LU10" s="199" t="n"/>
+      <c r="LU10" s="199" t="inlineStr"/>
       <c r="LV10" s="199" t="n"/>
       <c r="LW10" s="199" t="n"/>
       <c r="LX10" s="199" t="n"/>
@@ -8743,7 +8769,7 @@
       <c r="LR11" s="199" t="n"/>
       <c r="LS11" s="199" t="n"/>
       <c r="LT11" s="199" t="n"/>
-      <c r="LU11" s="199" t="n"/>
+      <c r="LU11" s="199" t="inlineStr"/>
       <c r="LV11" s="199" t="n"/>
       <c r="LW11" s="199" t="n"/>
       <c r="LX11" s="199" t="n"/>
@@ -9287,7 +9313,7 @@
       <c r="LR12" s="104" t="n"/>
       <c r="LS12" s="104" t="n"/>
       <c r="LT12" s="104" t="n"/>
-      <c r="LU12" s="104" t="n"/>
+      <c r="LU12" s="104" t="inlineStr"/>
       <c r="LV12" s="104" t="n"/>
       <c r="LW12" s="104" t="n"/>
       <c r="LX12" s="104" t="n"/>
@@ -9805,7 +9831,7 @@
       <c r="LR13" s="199" t="n"/>
       <c r="LS13" s="199" t="n"/>
       <c r="LT13" s="199" t="n"/>
-      <c r="LU13" s="199" t="n"/>
+      <c r="LU13" s="199" t="inlineStr"/>
       <c r="LV13" s="199" t="n"/>
       <c r="LW13" s="199" t="n"/>
       <c r="LX13" s="199" t="n"/>
@@ -10253,7 +10279,7 @@
       <c r="LR14" s="104" t="n"/>
       <c r="LS14" s="104" t="n"/>
       <c r="LT14" s="104" t="n"/>
-      <c r="LU14" s="104" t="n"/>
+      <c r="LU14" s="104" t="inlineStr"/>
       <c r="LV14" s="104" t="n"/>
       <c r="LW14" s="104" t="n"/>
       <c r="LX14" s="104" t="n"/>
@@ -10815,7 +10841,7 @@
       <c r="LR15" s="199" t="n"/>
       <c r="LS15" s="199" t="n"/>
       <c r="LT15" s="199" t="n"/>
-      <c r="LU15" s="199" t="n"/>
+      <c r="LU15" s="199" t="inlineStr"/>
       <c r="LV15" s="199" t="n"/>
       <c r="LW15" s="199" t="n"/>
       <c r="LX15" s="199" t="n"/>
@@ -11265,7 +11291,7 @@
       <c r="LR16" s="104" t="n"/>
       <c r="LS16" s="104" t="n"/>
       <c r="LT16" s="104" t="n"/>
-      <c r="LU16" s="104" t="n"/>
+      <c r="LU16" s="104" t="inlineStr"/>
       <c r="LV16" s="104" t="n"/>
       <c r="LW16" s="104" t="n"/>
       <c r="LX16" s="104" t="n"/>
@@ -11821,7 +11847,7 @@
       <c r="LR17" s="104" t="n"/>
       <c r="LS17" s="104" t="n"/>
       <c r="LT17" s="104" t="n"/>
-      <c r="LU17" s="104" t="n"/>
+      <c r="LU17" s="104" t="inlineStr"/>
       <c r="LV17" s="104" t="n"/>
       <c r="LW17" s="104" t="n"/>
       <c r="LX17" s="104" t="n"/>
@@ -12377,7 +12403,7 @@
       <c r="LR18" s="104" t="n"/>
       <c r="LS18" s="104" t="n"/>
       <c r="LT18" s="104" t="n"/>
-      <c r="LU18" s="104" t="n"/>
+      <c r="LU18" s="104" t="inlineStr"/>
       <c r="LV18" s="104" t="n"/>
       <c r="LW18" s="104" t="n"/>
       <c r="LX18" s="104" t="n"/>
@@ -12484,13 +12510,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -12882,24 +12908,46 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="104" t="inlineStr">
         <is>
           <t>Fart</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="104" t="inlineStr">
         <is>
           <t>poopy</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="104" t="inlineStr">
         <is>
           <t>special</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="104" t="inlineStr">
         <is>
           <t>Today</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="104" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B20" s="104" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="C20" s="104" t="inlineStr">
+        <is>
+          <t>89874</t>
+        </is>
+      </c>
+      <c r="D20" s="104" t="inlineStr">
+        <is>
+          <t>78</t>
         </is>
       </c>
     </row>
@@ -12922,7 +12970,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -13167,7 +13215,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14868,7 +14916,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
Working on the truck percentage entry field.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -5177,7 +5177,11 @@
           <t>oppo</t>
         </is>
       </c>
-      <c r="LU3" s="104" t="inlineStr"/>
+      <c r="LU3" s="104" t="inlineStr">
+        <is>
+          <t>489</t>
+        </is>
+      </c>
       <c r="LV3" s="104" t="n"/>
       <c r="LW3" s="104" t="n"/>
       <c r="LX3" s="104" t="n"/>
@@ -5737,7 +5741,11 @@
           <t>popo</t>
         </is>
       </c>
-      <c r="LU4" s="104" t="inlineStr"/>
+      <c r="LU4" s="104" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
       <c r="LV4" s="104" t="n"/>
       <c r="LW4" s="104" t="n"/>
       <c r="LX4" s="104" t="n"/>
@@ -6275,7 +6283,11 @@
           <t>opop</t>
         </is>
       </c>
-      <c r="LU5" s="104" t="inlineStr"/>
+      <c r="LU5" s="104" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
       <c r="LV5" s="104" t="n"/>
       <c r="LW5" s="104" t="n"/>
       <c r="LX5" s="104" t="n"/>
@@ -6807,7 +6819,11 @@
           <t>ooop</t>
         </is>
       </c>
-      <c r="LU6" s="104" t="inlineStr"/>
+      <c r="LU6" s="104" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
       <c r="LV6" s="104" t="n"/>
       <c r="LW6" s="104" t="n"/>
       <c r="LX6" s="104" t="n"/>
@@ -7159,7 +7175,11 @@
           <t>bii</t>
         </is>
       </c>
-      <c r="LU7" s="104" t="inlineStr"/>
+      <c r="LU7" s="104" t="inlineStr">
+        <is>
+          <t>76485486</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="106">
       <c r="A8" s="104" t="n"/>
@@ -7690,7 +7710,11 @@
       <c r="LR8" s="104" t="n"/>
       <c r="LS8" s="104" t="n"/>
       <c r="LT8" s="104" t="n"/>
-      <c r="LU8" s="104" t="inlineStr"/>
+      <c r="LU8" s="104" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
       <c r="LV8" s="104" t="n"/>
       <c r="LW8" s="104" t="n"/>
       <c r="LX8" s="104" t="n"/>
@@ -7844,7 +7868,11 @@
           <t>h</t>
         </is>
       </c>
-      <c r="LU9" s="104" t="inlineStr"/>
+      <c r="LU9" s="104" t="inlineStr">
+        <is>
+          <t>486</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="106">
       <c r="A10" s="199" t="n"/>
@@ -8241,7 +8269,11 @@
       <c r="LR10" s="199" t="n"/>
       <c r="LS10" s="199" t="n"/>
       <c r="LT10" s="199" t="n"/>
-      <c r="LU10" s="199" t="inlineStr"/>
+      <c r="LU10" s="199" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
       <c r="LV10" s="199" t="n"/>
       <c r="LW10" s="199" t="n"/>
       <c r="LX10" s="199" t="n"/>
@@ -8769,7 +8801,11 @@
       <c r="LR11" s="199" t="n"/>
       <c r="LS11" s="199" t="n"/>
       <c r="LT11" s="199" t="n"/>
-      <c r="LU11" s="199" t="inlineStr"/>
+      <c r="LU11" s="199" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
       <c r="LV11" s="199" t="n"/>
       <c r="LW11" s="199" t="n"/>
       <c r="LX11" s="199" t="n"/>
@@ -9313,7 +9349,11 @@
       <c r="LR12" s="104" t="n"/>
       <c r="LS12" s="104" t="n"/>
       <c r="LT12" s="104" t="n"/>
-      <c r="LU12" s="104" t="inlineStr"/>
+      <c r="LU12" s="104" t="inlineStr">
+        <is>
+          <t>8668</t>
+        </is>
+      </c>
       <c r="LV12" s="104" t="n"/>
       <c r="LW12" s="104" t="n"/>
       <c r="LX12" s="104" t="n"/>
@@ -9831,7 +9871,11 @@
       <c r="LR13" s="199" t="n"/>
       <c r="LS13" s="199" t="n"/>
       <c r="LT13" s="199" t="n"/>
-      <c r="LU13" s="199" t="inlineStr"/>
+      <c r="LU13" s="199" t="inlineStr">
+        <is>
+          <t>4468</t>
+        </is>
+      </c>
       <c r="LV13" s="199" t="n"/>
       <c r="LW13" s="199" t="n"/>
       <c r="LX13" s="199" t="n"/>
@@ -10279,7 +10323,11 @@
       <c r="LR14" s="104" t="n"/>
       <c r="LS14" s="104" t="n"/>
       <c r="LT14" s="104" t="n"/>
-      <c r="LU14" s="104" t="inlineStr"/>
+      <c r="LU14" s="104" t="inlineStr">
+        <is>
+          <t>684</t>
+        </is>
+      </c>
       <c r="LV14" s="104" t="n"/>
       <c r="LW14" s="104" t="n"/>
       <c r="LX14" s="104" t="n"/>
@@ -10841,7 +10889,11 @@
       <c r="LR15" s="199" t="n"/>
       <c r="LS15" s="199" t="n"/>
       <c r="LT15" s="199" t="n"/>
-      <c r="LU15" s="199" t="inlineStr"/>
+      <c r="LU15" s="199" t="inlineStr">
+        <is>
+          <t>684</t>
+        </is>
+      </c>
       <c r="LV15" s="199" t="n"/>
       <c r="LW15" s="199" t="n"/>
       <c r="LX15" s="199" t="n"/>
@@ -11291,7 +11343,11 @@
       <c r="LR16" s="104" t="n"/>
       <c r="LS16" s="104" t="n"/>
       <c r="LT16" s="104" t="n"/>
-      <c r="LU16" s="104" t="inlineStr"/>
+      <c r="LU16" s="104" t="inlineStr">
+        <is>
+          <t>486</t>
+        </is>
+      </c>
       <c r="LV16" s="104" t="n"/>
       <c r="LW16" s="104" t="n"/>
       <c r="LX16" s="104" t="n"/>
@@ -11847,7 +11903,11 @@
       <c r="LR17" s="104" t="n"/>
       <c r="LS17" s="104" t="n"/>
       <c r="LT17" s="104" t="n"/>
-      <c r="LU17" s="104" t="inlineStr"/>
+      <c r="LU17" s="104" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
       <c r="LV17" s="104" t="n"/>
       <c r="LW17" s="104" t="n"/>
       <c r="LX17" s="104" t="n"/>
@@ -12403,7 +12463,11 @@
       <c r="LR18" s="104" t="n"/>
       <c r="LS18" s="104" t="n"/>
       <c r="LT18" s="104" t="n"/>
-      <c r="LU18" s="104" t="inlineStr"/>
+      <c r="LU18" s="104" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
       <c r="LV18" s="104" t="n"/>
       <c r="LW18" s="104" t="n"/>
       <c r="LX18" s="104" t="n"/>

</xml_diff>

<commit_message>
Truck fill percentage is working correctly now. Just have to add the symbol.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -2910,7 +2910,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -4611,10 +4611,14 @@
       </c>
       <c r="LU2" s="104" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="LV2" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV2" s="104" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="LW2" s="104" t="n"/>
       <c r="LX2" s="104" t="n"/>
       <c r="LY2" s="104" t="n"/>
@@ -5179,10 +5183,14 @@
       </c>
       <c r="LU3" s="104" t="inlineStr">
         <is>
-          <t>489</t>
-        </is>
-      </c>
-      <c r="LV3" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV3" s="104" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
       <c r="LW3" s="104" t="n"/>
       <c r="LX3" s="104" t="n"/>
       <c r="LY3" s="104" t="n"/>
@@ -5743,10 +5751,14 @@
       </c>
       <c r="LU4" s="104" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="LV4" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV4" s="104" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
       <c r="LW4" s="104" t="n"/>
       <c r="LX4" s="104" t="n"/>
       <c r="LY4" s="104" t="n"/>
@@ -6285,10 +6297,14 @@
       </c>
       <c r="LU5" s="104" t="inlineStr">
         <is>
-          <t>68</t>
-        </is>
-      </c>
-      <c r="LV5" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV5" s="104" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="LW5" s="104" t="n"/>
       <c r="LX5" s="104" t="n"/>
       <c r="LY5" s="104" t="n"/>
@@ -6821,10 +6837,14 @@
       </c>
       <c r="LU6" s="104" t="inlineStr">
         <is>
-          <t>65</t>
-        </is>
-      </c>
-      <c r="LV6" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV6" s="104" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
       <c r="LW6" s="104" t="n"/>
       <c r="LX6" s="104" t="n"/>
       <c r="LY6" s="104" t="n"/>
@@ -7177,7 +7197,12 @@
       </c>
       <c r="LU7" s="104" t="inlineStr">
         <is>
-          <t>76485486</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV7" s="104" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -7712,10 +7737,14 @@
       <c r="LT8" s="104" t="n"/>
       <c r="LU8" s="104" t="inlineStr">
         <is>
-          <t>86</t>
-        </is>
-      </c>
-      <c r="LV8" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV8" s="104" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="LW8" s="104" t="n"/>
       <c r="LX8" s="104" t="n"/>
       <c r="LY8" s="104" t="n"/>
@@ -7870,7 +7899,12 @@
       </c>
       <c r="LU9" s="104" t="inlineStr">
         <is>
-          <t>486</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV9" s="104" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -8271,10 +8305,14 @@
       <c r="LT10" s="199" t="n"/>
       <c r="LU10" s="199" t="inlineStr">
         <is>
-          <t>864</t>
-        </is>
-      </c>
-      <c r="LV10" s="199" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV10" s="199" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
       <c r="LW10" s="199" t="n"/>
       <c r="LX10" s="199" t="n"/>
       <c r="LY10" s="199" t="n"/>
@@ -8803,10 +8841,14 @@
       <c r="LT11" s="199" t="n"/>
       <c r="LU11" s="199" t="inlineStr">
         <is>
-          <t>864</t>
-        </is>
-      </c>
-      <c r="LV11" s="199" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV11" s="199" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="LW11" s="199" t="n"/>
       <c r="LX11" s="199" t="n"/>
       <c r="LY11" s="199" t="n"/>
@@ -9351,10 +9393,14 @@
       <c r="LT12" s="104" t="n"/>
       <c r="LU12" s="104" t="inlineStr">
         <is>
-          <t>8668</t>
-        </is>
-      </c>
-      <c r="LV12" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV12" s="104" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="LW12" s="104" t="n"/>
       <c r="LX12" s="104" t="n"/>
       <c r="LY12" s="104" t="n"/>
@@ -9873,10 +9919,14 @@
       <c r="LT13" s="199" t="n"/>
       <c r="LU13" s="199" t="inlineStr">
         <is>
-          <t>4468</t>
-        </is>
-      </c>
-      <c r="LV13" s="199" t="n"/>
+          <t>7.69</t>
+        </is>
+      </c>
+      <c r="LV13" s="199" t="inlineStr">
+        <is>
+          <t>7.6923076923076925</t>
+        </is>
+      </c>
       <c r="LW13" s="199" t="n"/>
       <c r="LX13" s="199" t="n"/>
       <c r="LY13" s="199" t="n"/>
@@ -10325,10 +10375,14 @@
       <c r="LT14" s="104" t="n"/>
       <c r="LU14" s="104" t="inlineStr">
         <is>
-          <t>684</t>
-        </is>
-      </c>
-      <c r="LV14" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV14" s="104" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
       <c r="LW14" s="104" t="n"/>
       <c r="LX14" s="104" t="n"/>
       <c r="LY14" s="104" t="n"/>
@@ -10891,10 +10945,14 @@
       <c r="LT15" s="199" t="n"/>
       <c r="LU15" s="199" t="inlineStr">
         <is>
-          <t>684</t>
-        </is>
-      </c>
-      <c r="LV15" s="199" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV15" s="199" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
       <c r="LW15" s="199" t="n"/>
       <c r="LX15" s="199" t="n"/>
       <c r="LY15" s="199" t="n"/>
@@ -11345,10 +11403,14 @@
       <c r="LT16" s="104" t="n"/>
       <c r="LU16" s="104" t="inlineStr">
         <is>
-          <t>486</t>
-        </is>
-      </c>
-      <c r="LV16" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV16" s="104" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="LW16" s="104" t="n"/>
       <c r="LX16" s="104" t="n"/>
       <c r="LY16" s="104" t="n"/>
@@ -11905,10 +11967,14 @@
       <c r="LT17" s="104" t="n"/>
       <c r="LU17" s="104" t="inlineStr">
         <is>
-          <t>864</t>
-        </is>
-      </c>
-      <c r="LV17" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV17" s="104" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
       <c r="LW17" s="104" t="n"/>
       <c r="LX17" s="104" t="n"/>
       <c r="LY17" s="104" t="n"/>
@@ -12465,10 +12531,14 @@
       <c r="LT18" s="104" t="n"/>
       <c r="LU18" s="104" t="inlineStr">
         <is>
-          <t>84</t>
-        </is>
-      </c>
-      <c r="LV18" s="104" t="n"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="LV18" s="104" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
       <c r="LW18" s="104" t="n"/>
       <c r="LX18" s="104" t="n"/>
       <c r="LY18" s="104" t="n"/>
@@ -12580,7 +12650,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -13034,7 +13104,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -13279,7 +13349,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14980,7 +15050,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
JUST NEED TO PUSH AND PULL FROM GIT
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -2684,9 +2684,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="H19:Q19"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="F5:H5"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -2910,7 +2910,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -5177,7 +5177,11 @@
           <t>oppo</t>
         </is>
       </c>
-      <c r="LU3" s="104" t="inlineStr"/>
+      <c r="LU3" s="104" t="inlineStr">
+        <is>
+          <t>ui</t>
+        </is>
+      </c>
       <c r="LV3" s="104" t="n"/>
       <c r="LW3" s="104" t="n"/>
       <c r="LX3" s="104" t="n"/>
@@ -5737,7 +5741,11 @@
           <t>popo</t>
         </is>
       </c>
-      <c r="LU4" s="104" t="inlineStr"/>
+      <c r="LU4" s="104" t="inlineStr">
+        <is>
+          <t>ui</t>
+        </is>
+      </c>
       <c r="LV4" s="104" t="n"/>
       <c r="LW4" s="104" t="n"/>
       <c r="LX4" s="104" t="n"/>
@@ -6275,7 +6283,11 @@
           <t>opop</t>
         </is>
       </c>
-      <c r="LU5" s="104" t="inlineStr"/>
+      <c r="LU5" s="104" t="inlineStr">
+        <is>
+          <t>ug</t>
+        </is>
+      </c>
       <c r="LV5" s="104" t="n"/>
       <c r="LW5" s="104" t="n"/>
       <c r="LX5" s="104" t="n"/>
@@ -6807,7 +6819,11 @@
           <t>ooop</t>
         </is>
       </c>
-      <c r="LU6" s="104" t="inlineStr"/>
+      <c r="LU6" s="104" t="inlineStr">
+        <is>
+          <t>iu</t>
+        </is>
+      </c>
       <c r="LV6" s="104" t="n"/>
       <c r="LW6" s="104" t="n"/>
       <c r="LX6" s="104" t="n"/>
@@ -7159,7 +7175,11 @@
           <t>bii</t>
         </is>
       </c>
-      <c r="LU7" s="104" t="inlineStr"/>
+      <c r="LU7" s="104" t="inlineStr">
+        <is>
+          <t>gui</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="106">
       <c r="A8" s="104" t="n"/>
@@ -7690,7 +7710,11 @@
       <c r="LR8" s="104" t="n"/>
       <c r="LS8" s="104" t="n"/>
       <c r="LT8" s="104" t="n"/>
-      <c r="LU8" s="104" t="inlineStr"/>
+      <c r="LU8" s="104" t="inlineStr">
+        <is>
+          <t>ui</t>
+        </is>
+      </c>
       <c r="LV8" s="104" t="n"/>
       <c r="LW8" s="104" t="n"/>
       <c r="LX8" s="104" t="n"/>
@@ -7844,7 +7868,11 @@
           <t>h</t>
         </is>
       </c>
-      <c r="LU9" s="104" t="inlineStr"/>
+      <c r="LU9" s="104" t="inlineStr">
+        <is>
+          <t>ui</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="106">
       <c r="A10" s="199" t="n"/>
@@ -8241,7 +8269,11 @@
       <c r="LR10" s="199" t="n"/>
       <c r="LS10" s="199" t="n"/>
       <c r="LT10" s="199" t="n"/>
-      <c r="LU10" s="199" t="inlineStr"/>
+      <c r="LU10" s="199" t="inlineStr">
+        <is>
+          <t>lg</t>
+        </is>
+      </c>
       <c r="LV10" s="199" t="n"/>
       <c r="LW10" s="199" t="n"/>
       <c r="LX10" s="199" t="n"/>
@@ -8769,7 +8801,11 @@
       <c r="LR11" s="199" t="n"/>
       <c r="LS11" s="199" t="n"/>
       <c r="LT11" s="199" t="n"/>
-      <c r="LU11" s="199" t="inlineStr"/>
+      <c r="LU11" s="199" t="inlineStr">
+        <is>
+          <t>iu</t>
+        </is>
+      </c>
       <c r="LV11" s="199" t="n"/>
       <c r="LW11" s="199" t="n"/>
       <c r="LX11" s="199" t="n"/>
@@ -9313,7 +9349,11 @@
       <c r="LR12" s="104" t="n"/>
       <c r="LS12" s="104" t="n"/>
       <c r="LT12" s="104" t="n"/>
-      <c r="LU12" s="104" t="inlineStr"/>
+      <c r="LU12" s="104" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
       <c r="LV12" s="104" t="n"/>
       <c r="LW12" s="104" t="n"/>
       <c r="LX12" s="104" t="n"/>
@@ -9831,7 +9871,11 @@
       <c r="LR13" s="199" t="n"/>
       <c r="LS13" s="199" t="n"/>
       <c r="LT13" s="199" t="n"/>
-      <c r="LU13" s="199" t="inlineStr"/>
+      <c r="LU13" s="199" t="inlineStr">
+        <is>
+          <t>iuy</t>
+        </is>
+      </c>
       <c r="LV13" s="199" t="n"/>
       <c r="LW13" s="199" t="n"/>
       <c r="LX13" s="199" t="n"/>
@@ -10279,7 +10323,11 @@
       <c r="LR14" s="104" t="n"/>
       <c r="LS14" s="104" t="n"/>
       <c r="LT14" s="104" t="n"/>
-      <c r="LU14" s="104" t="inlineStr"/>
+      <c r="LU14" s="104" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
       <c r="LV14" s="104" t="n"/>
       <c r="LW14" s="104" t="n"/>
       <c r="LX14" s="104" t="n"/>
@@ -10841,7 +10889,11 @@
       <c r="LR15" s="199" t="n"/>
       <c r="LS15" s="199" t="n"/>
       <c r="LT15" s="199" t="n"/>
-      <c r="LU15" s="199" t="inlineStr"/>
+      <c r="LU15" s="199" t="inlineStr">
+        <is>
+          <t>uk</t>
+        </is>
+      </c>
       <c r="LV15" s="199" t="n"/>
       <c r="LW15" s="199" t="n"/>
       <c r="LX15" s="199" t="n"/>
@@ -11291,7 +11343,11 @@
       <c r="LR16" s="104" t="n"/>
       <c r="LS16" s="104" t="n"/>
       <c r="LT16" s="104" t="n"/>
-      <c r="LU16" s="104" t="inlineStr"/>
+      <c r="LU16" s="104" t="inlineStr">
+        <is>
+          <t>giu</t>
+        </is>
+      </c>
       <c r="LV16" s="104" t="n"/>
       <c r="LW16" s="104" t="n"/>
       <c r="LX16" s="104" t="n"/>
@@ -11847,7 +11903,11 @@
       <c r="LR17" s="104" t="n"/>
       <c r="LS17" s="104" t="n"/>
       <c r="LT17" s="104" t="n"/>
-      <c r="LU17" s="104" t="inlineStr"/>
+      <c r="LU17" s="104" t="inlineStr">
+        <is>
+          <t>gjk</t>
+        </is>
+      </c>
       <c r="LV17" s="104" t="n"/>
       <c r="LW17" s="104" t="n"/>
       <c r="LX17" s="104" t="n"/>
@@ -12403,7 +12463,11 @@
       <c r="LR18" s="104" t="n"/>
       <c r="LS18" s="104" t="n"/>
       <c r="LT18" s="104" t="n"/>
-      <c r="LU18" s="104" t="inlineStr"/>
+      <c r="LU18" s="104" t="inlineStr">
+        <is>
+          <t>kjhg</t>
+        </is>
+      </c>
       <c r="LV18" s="104" t="n"/>
       <c r="LW18" s="104" t="n"/>
       <c r="LX18" s="104" t="n"/>
@@ -12516,7 +12580,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -12970,7 +13034,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -13215,7 +13279,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14916,7 +14980,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
edited code for clarity and added code for new date rows.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -1644,7 +1644,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="104" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="104" min="2" max="2"/>
@@ -2684,9 +2684,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="H19:Q19"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="H19:Q19"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -2895,7 +2895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -2910,7 +2910,7 @@
       <selection pane="bottomRight" activeCell="FQ2" activeCellId="0" sqref="FQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="104" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="104" min="135" max="139"/>
@@ -4029,7 +4029,11 @@
           <t>Days without Incident</t>
         </is>
       </c>
-      <c r="C2" s="104" t="n"/>
+      <c r="C2" s="104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="D2" s="104" t="n"/>
       <c r="E2" s="104" t="n"/>
       <c r="F2" s="104" t="n"/>
@@ -4657,7 +4661,11 @@
           <t>Haz ID's</t>
         </is>
       </c>
-      <c r="C3" s="104" t="inlineStr"/>
+      <c r="C3" s="104" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
       <c r="D3" s="104" t="n"/>
       <c r="E3" s="104" t="n"/>
       <c r="F3" s="104" t="n"/>
@@ -5225,7 +5233,11 @@
           <t>Safety Gemba Walk</t>
         </is>
       </c>
-      <c r="C4" s="104" t="inlineStr"/>
+      <c r="C4" s="104" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
       <c r="D4" s="104" t="n"/>
       <c r="E4" s="104" t="n"/>
       <c r="F4" s="104" t="n"/>
@@ -5789,7 +5801,11 @@
           <t>7S (Zone 26)</t>
         </is>
       </c>
-      <c r="C5" s="104" t="inlineStr"/>
+      <c r="C5" s="104" t="inlineStr">
+        <is>
+          <t>564</t>
+        </is>
+      </c>
       <c r="D5" s="104" t="n"/>
       <c r="E5" s="104" t="n"/>
       <c r="F5" s="104" t="n"/>
@@ -6331,7 +6347,11 @@
           <t>7S (Zone 51)</t>
         </is>
       </c>
-      <c r="C6" s="104" t="inlineStr"/>
+      <c r="C6" s="104" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
       <c r="D6" s="104" t="n"/>
       <c r="E6" s="104" t="n"/>
       <c r="F6" s="104" t="n"/>
@@ -6867,7 +6887,11 @@
           <t>Errors</t>
         </is>
       </c>
-      <c r="C7" s="199" t="n"/>
+      <c r="C7" s="199" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
       <c r="D7" s="199" t="n"/>
       <c r="E7" s="199" t="n"/>
       <c r="F7" s="199" t="n"/>
@@ -7188,7 +7212,11 @@
           <t>PCD Returns</t>
         </is>
       </c>
-      <c r="C8" s="104" t="n"/>
+      <c r="C8" s="104" t="inlineStr">
+        <is>
+          <t>1894</t>
+        </is>
+      </c>
       <c r="D8" s="104" t="n"/>
       <c r="E8" s="104" t="n"/>
       <c r="F8" s="104" t="n"/>
@@ -7757,6 +7785,11 @@
           <t>Jobs on Hold</t>
         </is>
       </c>
+      <c r="C9" s="104" t="inlineStr">
+        <is>
+          <t>586</t>
+        </is>
+      </c>
       <c r="DC9" s="104" t="n">
         <v>0</v>
       </c>
@@ -7881,7 +7914,11 @@
           <t>Productivity</t>
         </is>
       </c>
-      <c r="C10" s="199" t="n"/>
+      <c r="C10" s="199" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
       <c r="D10" s="199" t="n"/>
       <c r="E10" s="199" t="n"/>
       <c r="F10" s="199" t="n"/>
@@ -8317,7 +8354,11 @@
           <t>OTIF %</t>
         </is>
       </c>
-      <c r="C11" s="199" t="n"/>
+      <c r="C11" s="199" t="inlineStr">
+        <is>
+          <t>564</t>
+        </is>
+      </c>
       <c r="D11" s="199" t="n"/>
       <c r="E11" s="199" t="n"/>
       <c r="F11" s="199" t="n"/>
@@ -8849,7 +8890,11 @@
           <t>Huddles</t>
         </is>
       </c>
-      <c r="C12" s="104" t="n"/>
+      <c r="C12" s="104" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
       <c r="D12" s="104" t="n"/>
       <c r="E12" s="104" t="n"/>
       <c r="F12" s="104" t="n"/>
@@ -9397,7 +9442,11 @@
           <t>Truck Fill %</t>
         </is>
       </c>
-      <c r="C13" s="199" t="n"/>
+      <c r="C13" s="199" t="inlineStr">
+        <is>
+          <t>19.23%</t>
+        </is>
+      </c>
       <c r="D13" s="199" t="n"/>
       <c r="E13" s="199" t="n"/>
       <c r="F13" s="199" t="n"/>
@@ -9919,7 +9968,11 @@
           <t>Recognitions</t>
         </is>
       </c>
-      <c r="C14" s="104" t="n"/>
+      <c r="C14" s="104" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
       <c r="D14" s="104" t="n"/>
       <c r="E14" s="104" t="n"/>
       <c r="F14" s="104" t="n"/>
@@ -10371,7 +10424,11 @@
           <t>MC Compliance</t>
         </is>
       </c>
-      <c r="C15" s="199" t="n"/>
+      <c r="C15" s="199" t="inlineStr">
+        <is>
+          <t>489</t>
+        </is>
+      </c>
       <c r="D15" s="199" t="n"/>
       <c r="E15" s="199" t="n"/>
       <c r="F15" s="199" t="n"/>
@@ -10937,7 +10994,11 @@
           <t>Cost Savings</t>
         </is>
       </c>
-      <c r="C16" s="104" t="n"/>
+      <c r="C16" s="104" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
       <c r="D16" s="104" t="n"/>
       <c r="E16" s="104" t="n"/>
       <c r="F16" s="104" t="n"/>
@@ -11391,7 +11452,11 @@
           <t>Rever's</t>
         </is>
       </c>
-      <c r="C17" s="104" t="n"/>
+      <c r="C17" s="104" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="D17" s="104" t="n"/>
       <c r="E17" s="104" t="n"/>
       <c r="F17" s="104" t="n"/>
@@ -11951,7 +12016,11 @@
           <t>Project's</t>
         </is>
       </c>
-      <c r="C18" s="104" t="n"/>
+      <c r="C18" s="104" t="inlineStr">
+        <is>
+          <t>854</t>
+        </is>
+      </c>
       <c r="D18" s="104" t="n"/>
       <c r="E18" s="104" t="n"/>
       <c r="F18" s="104" t="n"/>
@@ -12564,7 +12633,7 @@
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -12580,7 +12649,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="104" min="1" max="1"/>
     <col width="17" customWidth="1" style="104" min="2" max="2"/>
@@ -13034,7 +13103,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="211" min="1" max="1"/>
     <col width="11" customWidth="1" style="211" min="2" max="2"/>
@@ -13279,7 +13348,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="217" min="2" max="2"/>
     <col width="12" customWidth="1" style="217" min="3" max="3"/>
@@ -14980,7 +15049,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="217" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="217" min="5" max="5"/>

</xml_diff>

<commit_message>
Working on the Log
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -3269,7 +3269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:NL27"/>
+  <dimension ref="A1:NJ27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="FH2" activePane="bottomRight" state="frozen"/>
@@ -4408,14 +4408,6 @@
       <c r="NJ1" s="240" t="n">
         <v>45663</v>
       </c>
-      <c r="NK1" s="240" t="n">
-        <v>45663</v>
-      </c>
-      <c r="NL1" s="108" t="inlineStr">
-        <is>
-          <t>01/06/2025</t>
-        </is>
-      </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="110">
       <c r="B2" s="204" t="inlineStr">
@@ -4908,7 +4900,7 @@
       <c r="FX2" s="108" t="n">
         <v>60</v>
       </c>
-      <c r="NL2" s="108" t="inlineStr">
+      <c r="NJ2" s="108" t="inlineStr">
         <is>
           <t>41</t>
         </is>
@@ -5181,11 +5173,7 @@
       <c r="FO3" s="108" t="n">
         <v>0</v>
       </c>
-      <c r="NL3" s="108" t="inlineStr">
-        <is>
-          <t>496</t>
-        </is>
-      </c>
+      <c r="NJ3" s="108" t="inlineStr"/>
     </row>
     <row r="4" ht="15" customHeight="1" s="110">
       <c r="B4" s="204" t="inlineStr">
@@ -5448,11 +5436,7 @@
       <c r="FO4" s="108" t="n">
         <v>1</v>
       </c>
-      <c r="NL4" s="108" t="inlineStr">
-        <is>
-          <t>684</t>
-        </is>
-      </c>
+      <c r="NJ4" s="108" t="inlineStr"/>
     </row>
     <row r="5" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B5" s="206" t="inlineStr">
@@ -5734,11 +5718,7 @@
       <c r="FO5" s="205" t="n">
         <v>4.03</v>
       </c>
-      <c r="NL5" s="108" t="inlineStr">
-        <is>
-          <t>658</t>
-        </is>
-      </c>
+      <c r="NJ5" s="108" t="inlineStr"/>
     </row>
     <row r="6" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B6" s="206" t="inlineStr">
@@ -6011,11 +5991,7 @@
       <c r="FO6" s="205" t="n">
         <v>3.1</v>
       </c>
-      <c r="NL6" s="108" t="inlineStr">
-        <is>
-          <t>416</t>
-        </is>
-      </c>
+      <c r="NJ6" s="108" t="inlineStr"/>
     </row>
     <row r="7" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="A7" s="208" t="n"/>
@@ -6322,11 +6298,7 @@
       <c r="FO7" s="207" t="n">
         <v>1</v>
       </c>
-      <c r="NL7" s="108" t="inlineStr">
-        <is>
-          <t>185</t>
-        </is>
-      </c>
+      <c r="NJ7" s="108" t="inlineStr"/>
     </row>
     <row r="8" ht="15" customHeight="1" s="110">
       <c r="B8" s="210" t="inlineStr">
@@ -6604,11 +6576,7 @@
       <c r="FO8" s="207" t="n">
         <v>1</v>
       </c>
-      <c r="NL8" s="108" t="inlineStr">
-        <is>
-          <t>8569</t>
-        </is>
-      </c>
+      <c r="NJ8" s="108" t="inlineStr"/>
     </row>
     <row r="9" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="B9" s="211" t="inlineStr">
@@ -6712,11 +6680,7 @@
       <c r="FO9" s="207" t="n">
         <v>0</v>
       </c>
-      <c r="NL9" s="108" t="inlineStr">
-        <is>
-          <t>651</t>
-        </is>
-      </c>
+      <c r="NJ9" s="108" t="inlineStr"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="110">
       <c r="A10" s="208" t="n"/>
@@ -7357,11 +7321,7 @@
       <c r="NB10" s="208" t="n"/>
       <c r="NC10" s="208" t="n"/>
       <c r="ND10" s="208" t="n"/>
-      <c r="NL10" s="108" t="inlineStr">
-        <is>
-          <t>658</t>
-        </is>
-      </c>
+      <c r="NJ10" s="108" t="inlineStr"/>
     </row>
     <row r="11" ht="15" customHeight="1" s="110">
       <c r="A11" s="208" t="n"/>
@@ -7878,11 +7838,7 @@
       <c r="NB11" s="208" t="n"/>
       <c r="NC11" s="208" t="n"/>
       <c r="ND11" s="208" t="n"/>
-      <c r="NL11" s="108" t="inlineStr">
-        <is>
-          <t>516</t>
-        </is>
-      </c>
+      <c r="NJ11" s="108" t="inlineStr"/>
     </row>
     <row r="12" ht="15" customHeight="1" s="110">
       <c r="A12" s="207" t="n"/>
@@ -8431,11 +8387,7 @@
       <c r="NB12" s="207" t="n"/>
       <c r="NC12" s="207" t="n"/>
       <c r="ND12" s="207" t="n"/>
-      <c r="NL12" s="108" t="inlineStr">
-        <is>
-          <t>651</t>
-        </is>
-      </c>
+      <c r="NJ12" s="108" t="inlineStr"/>
     </row>
     <row r="13" ht="15" customHeight="1" s="110">
       <c r="A13" s="208" t="n"/>
@@ -9002,9 +8954,9 @@
       <c r="NB13" s="208" t="n"/>
       <c r="NC13" s="208" t="n"/>
       <c r="ND13" s="208" t="n"/>
-      <c r="NL13" s="108" t="inlineStr">
-        <is>
-          <t>65</t>
+      <c r="NJ13" s="108" t="inlineStr">
+        <is>
+          <t>15.38%</t>
         </is>
       </c>
     </row>
@@ -9107,11 +9059,7 @@
       <c r="FO14" s="207" t="n">
         <v>0</v>
       </c>
-      <c r="NL14" s="108" t="inlineStr">
-        <is>
-          <t>6581</t>
-        </is>
-      </c>
+      <c r="NJ14" s="108" t="inlineStr"/>
     </row>
     <row r="15" ht="15" customHeight="1" s="110">
       <c r="A15" s="208" t="n"/>
@@ -9662,11 +9610,7 @@
       <c r="NB15" s="208" t="n"/>
       <c r="NC15" s="208" t="n"/>
       <c r="ND15" s="208" t="n"/>
-      <c r="NL15" s="108" t="inlineStr">
-        <is>
-          <t>1958</t>
-        </is>
-      </c>
+      <c r="NJ15" s="108" t="inlineStr"/>
     </row>
     <row r="16" ht="15" customHeight="1" s="110">
       <c r="B16" s="215" t="inlineStr">
@@ -9770,11 +9714,7 @@
       <c r="FO16" s="216" t="n">
         <v>1735.5</v>
       </c>
-      <c r="NL16" s="108" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
+      <c r="NJ16" s="108" t="inlineStr"/>
     </row>
     <row r="17" ht="15" customHeight="1" s="110">
       <c r="B17" s="215" t="inlineStr">
@@ -10037,11 +9977,7 @@
       <c r="FO17" s="108" t="n">
         <v>0</v>
       </c>
-      <c r="NL17" s="108" t="inlineStr">
-        <is>
-          <t>56561</t>
-        </is>
-      </c>
+      <c r="NJ17" s="108" t="inlineStr"/>
     </row>
     <row r="18" ht="15" customHeight="1" s="110">
       <c r="B18" s="215" t="inlineStr">
@@ -10304,11 +10240,7 @@
       <c r="FO18" s="108" t="n">
         <v>5</v>
       </c>
-      <c r="NL18" s="108" t="inlineStr">
-        <is>
-          <t>4156</t>
-        </is>
-      </c>
+      <c r="NJ18" s="108" t="inlineStr"/>
     </row>
     <row r="19" ht="15" customHeight="1" s="110">
       <c r="B19" s="108" t="inlineStr">

</xml_diff>

<commit_message>
Added a text file to keep track of what I want to add and work on.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -3053,9 +3053,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="H19:Q19"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="F5:H5"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -3269,7 +3269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:NJ27"/>
+  <dimension ref="A1:NP27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="FH2" activePane="bottomRight" state="frozen"/>
@@ -4408,6 +4408,24 @@
       <c r="NJ1" s="240" t="n">
         <v>45663</v>
       </c>
+      <c r="NK1" s="240" t="n">
+        <v>45664</v>
+      </c>
+      <c r="NL1" s="240" t="n">
+        <v>45665</v>
+      </c>
+      <c r="NM1" s="240" t="n">
+        <v>45666</v>
+      </c>
+      <c r="NN1" s="240" t="n">
+        <v>45667</v>
+      </c>
+      <c r="NO1" s="240" t="n">
+        <v>45668</v>
+      </c>
+      <c r="NP1" s="240" t="n">
+        <v>45669</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="110">
       <c r="B2" s="204" t="inlineStr">
@@ -4905,6 +4923,21 @@
           <t>41</t>
         </is>
       </c>
+      <c r="NN2" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="NO2" s="108" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="NP2" s="108" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="110">
       <c r="B3" s="204" t="inlineStr">
@@ -5174,6 +5207,9 @@
         <v>0</v>
       </c>
       <c r="NJ3" s="108" t="inlineStr"/>
+      <c r="NN3" t="inlineStr"/>
+      <c r="NO3" s="108" t="inlineStr"/>
+      <c r="NP3" s="108" t="inlineStr"/>
     </row>
     <row r="4" ht="15" customHeight="1" s="110">
       <c r="B4" s="204" t="inlineStr">
@@ -5437,6 +5473,9 @@
         <v>1</v>
       </c>
       <c r="NJ4" s="108" t="inlineStr"/>
+      <c r="NN4" t="inlineStr"/>
+      <c r="NO4" s="108" t="inlineStr"/>
+      <c r="NP4" s="108" t="inlineStr"/>
     </row>
     <row r="5" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B5" s="206" t="inlineStr">
@@ -5719,6 +5758,9 @@
         <v>4.03</v>
       </c>
       <c r="NJ5" s="108" t="inlineStr"/>
+      <c r="NN5" t="inlineStr"/>
+      <c r="NO5" s="108" t="inlineStr"/>
+      <c r="NP5" s="108" t="inlineStr"/>
     </row>
     <row r="6" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B6" s="206" t="inlineStr">
@@ -5992,6 +6034,9 @@
         <v>3.1</v>
       </c>
       <c r="NJ6" s="108" t="inlineStr"/>
+      <c r="NN6" t="inlineStr"/>
+      <c r="NO6" s="108" t="inlineStr"/>
+      <c r="NP6" s="108" t="inlineStr"/>
     </row>
     <row r="7" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="A7" s="208" t="n"/>
@@ -6299,6 +6344,9 @@
         <v>1</v>
       </c>
       <c r="NJ7" s="108" t="inlineStr"/>
+      <c r="NN7" t="inlineStr"/>
+      <c r="NO7" s="108" t="inlineStr"/>
+      <c r="NP7" s="108" t="inlineStr"/>
     </row>
     <row r="8" ht="15" customHeight="1" s="110">
       <c r="B8" s="210" t="inlineStr">
@@ -6577,6 +6625,9 @@
         <v>1</v>
       </c>
       <c r="NJ8" s="108" t="inlineStr"/>
+      <c r="NN8" t="inlineStr"/>
+      <c r="NO8" s="108" t="inlineStr"/>
+      <c r="NP8" s="108" t="inlineStr"/>
     </row>
     <row r="9" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="B9" s="211" t="inlineStr">
@@ -6681,6 +6732,9 @@
         <v>0</v>
       </c>
       <c r="NJ9" s="108" t="inlineStr"/>
+      <c r="NN9" t="inlineStr"/>
+      <c r="NO9" s="108" t="inlineStr"/>
+      <c r="NP9" s="108" t="inlineStr"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="110">
       <c r="A10" s="208" t="n"/>
@@ -7322,6 +7376,9 @@
       <c r="NC10" s="208" t="n"/>
       <c r="ND10" s="208" t="n"/>
       <c r="NJ10" s="108" t="inlineStr"/>
+      <c r="NN10" t="inlineStr"/>
+      <c r="NO10" s="108" t="inlineStr"/>
+      <c r="NP10" s="108" t="inlineStr"/>
     </row>
     <row r="11" ht="15" customHeight="1" s="110">
       <c r="A11" s="208" t="n"/>
@@ -7839,6 +7896,9 @@
       <c r="NC11" s="208" t="n"/>
       <c r="ND11" s="208" t="n"/>
       <c r="NJ11" s="108" t="inlineStr"/>
+      <c r="NN11" t="inlineStr"/>
+      <c r="NO11" s="108" t="inlineStr"/>
+      <c r="NP11" s="108" t="inlineStr"/>
     </row>
     <row r="12" ht="15" customHeight="1" s="110">
       <c r="A12" s="207" t="n"/>
@@ -8388,6 +8448,9 @@
       <c r="NC12" s="207" t="n"/>
       <c r="ND12" s="207" t="n"/>
       <c r="NJ12" s="108" t="inlineStr"/>
+      <c r="NN12" t="inlineStr"/>
+      <c r="NO12" s="108" t="inlineStr"/>
+      <c r="NP12" s="108" t="inlineStr"/>
     </row>
     <row r="13" ht="15" customHeight="1" s="110">
       <c r="A13" s="208" t="n"/>
@@ -8959,6 +9022,21 @@
           <t>15.38%</t>
         </is>
       </c>
+      <c r="NN13" t="inlineStr">
+        <is>
+          <t>46.15%</t>
+        </is>
+      </c>
+      <c r="NO13" s="108" t="inlineStr">
+        <is>
+          <t>3.85%</t>
+        </is>
+      </c>
+      <c r="NP13" s="108" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="110">
       <c r="B14" s="213" t="inlineStr">
@@ -9060,6 +9138,9 @@
         <v>0</v>
       </c>
       <c r="NJ14" s="108" t="inlineStr"/>
+      <c r="NN14" t="inlineStr"/>
+      <c r="NO14" s="108" t="inlineStr"/>
+      <c r="NP14" s="108" t="inlineStr"/>
     </row>
     <row r="15" ht="15" customHeight="1" s="110">
       <c r="A15" s="208" t="n"/>
@@ -9611,6 +9692,9 @@
       <c r="NC15" s="208" t="n"/>
       <c r="ND15" s="208" t="n"/>
       <c r="NJ15" s="108" t="inlineStr"/>
+      <c r="NN15" t="inlineStr"/>
+      <c r="NO15" s="108" t="inlineStr"/>
+      <c r="NP15" s="108" t="inlineStr"/>
     </row>
     <row r="16" ht="15" customHeight="1" s="110">
       <c r="B16" s="215" t="inlineStr">
@@ -9715,6 +9799,9 @@
         <v>1735.5</v>
       </c>
       <c r="NJ16" s="108" t="inlineStr"/>
+      <c r="NN16" t="inlineStr"/>
+      <c r="NO16" s="108" t="inlineStr"/>
+      <c r="NP16" s="108" t="inlineStr"/>
     </row>
     <row r="17" ht="15" customHeight="1" s="110">
       <c r="B17" s="215" t="inlineStr">
@@ -9978,6 +10065,9 @@
         <v>0</v>
       </c>
       <c r="NJ17" s="108" t="inlineStr"/>
+      <c r="NN17" t="inlineStr"/>
+      <c r="NO17" s="108" t="inlineStr"/>
+      <c r="NP17" s="108" t="inlineStr"/>
     </row>
     <row r="18" ht="15" customHeight="1" s="110">
       <c r="B18" s="215" t="inlineStr">
@@ -10241,6 +10331,9 @@
         <v>5</v>
       </c>
       <c r="NJ18" s="108" t="inlineStr"/>
+      <c r="NN18" t="inlineStr"/>
+      <c r="NO18" s="108" t="inlineStr"/>
+      <c r="NP18" s="108" t="inlineStr"/>
     </row>
     <row r="19" ht="15" customHeight="1" s="110">
       <c r="B19" s="108" t="inlineStr">

</xml_diff>

<commit_message>
Trying to streamline and organize the script a bit.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -4923,7 +4923,7 @@
           <t>41</t>
         </is>
       </c>
-      <c r="NN2" t="inlineStr">
+      <c r="NN2" s="108" t="inlineStr">
         <is>
           <t>45</t>
         </is>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="NP2" s="108" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>dsfg</t>
         </is>
       </c>
     </row>
@@ -5207,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="NJ3" s="108" t="inlineStr"/>
-      <c r="NN3" t="inlineStr"/>
+      <c r="NN3" s="108" t="inlineStr"/>
       <c r="NO3" s="108" t="inlineStr"/>
       <c r="NP3" s="108" t="inlineStr"/>
     </row>
@@ -5473,7 +5473,7 @@
         <v>1</v>
       </c>
       <c r="NJ4" s="108" t="inlineStr"/>
-      <c r="NN4" t="inlineStr"/>
+      <c r="NN4" s="108" t="inlineStr"/>
       <c r="NO4" s="108" t="inlineStr"/>
       <c r="NP4" s="108" t="inlineStr"/>
     </row>
@@ -5758,7 +5758,7 @@
         <v>4.03</v>
       </c>
       <c r="NJ5" s="108" t="inlineStr"/>
-      <c r="NN5" t="inlineStr"/>
+      <c r="NN5" s="108" t="inlineStr"/>
       <c r="NO5" s="108" t="inlineStr"/>
       <c r="NP5" s="108" t="inlineStr"/>
     </row>
@@ -6034,7 +6034,7 @@
         <v>3.1</v>
       </c>
       <c r="NJ6" s="108" t="inlineStr"/>
-      <c r="NN6" t="inlineStr"/>
+      <c r="NN6" s="108" t="inlineStr"/>
       <c r="NO6" s="108" t="inlineStr"/>
       <c r="NP6" s="108" t="inlineStr"/>
     </row>
@@ -6344,7 +6344,7 @@
         <v>1</v>
       </c>
       <c r="NJ7" s="108" t="inlineStr"/>
-      <c r="NN7" t="inlineStr"/>
+      <c r="NN7" s="108" t="inlineStr"/>
       <c r="NO7" s="108" t="inlineStr"/>
       <c r="NP7" s="108" t="inlineStr"/>
     </row>
@@ -6625,7 +6625,7 @@
         <v>1</v>
       </c>
       <c r="NJ8" s="108" t="inlineStr"/>
-      <c r="NN8" t="inlineStr"/>
+      <c r="NN8" s="108" t="inlineStr"/>
       <c r="NO8" s="108" t="inlineStr"/>
       <c r="NP8" s="108" t="inlineStr"/>
     </row>
@@ -6732,7 +6732,7 @@
         <v>0</v>
       </c>
       <c r="NJ9" s="108" t="inlineStr"/>
-      <c r="NN9" t="inlineStr"/>
+      <c r="NN9" s="108" t="inlineStr"/>
       <c r="NO9" s="108" t="inlineStr"/>
       <c r="NP9" s="108" t="inlineStr"/>
     </row>
@@ -7376,7 +7376,7 @@
       <c r="NC10" s="208" t="n"/>
       <c r="ND10" s="208" t="n"/>
       <c r="NJ10" s="108" t="inlineStr"/>
-      <c r="NN10" t="inlineStr"/>
+      <c r="NN10" s="108" t="inlineStr"/>
       <c r="NO10" s="108" t="inlineStr"/>
       <c r="NP10" s="108" t="inlineStr"/>
     </row>
@@ -7896,7 +7896,7 @@
       <c r="NC11" s="208" t="n"/>
       <c r="ND11" s="208" t="n"/>
       <c r="NJ11" s="108" t="inlineStr"/>
-      <c r="NN11" t="inlineStr"/>
+      <c r="NN11" s="108" t="inlineStr"/>
       <c r="NO11" s="108" t="inlineStr"/>
       <c r="NP11" s="108" t="inlineStr"/>
     </row>
@@ -8448,7 +8448,7 @@
       <c r="NC12" s="207" t="n"/>
       <c r="ND12" s="207" t="n"/>
       <c r="NJ12" s="108" t="inlineStr"/>
-      <c r="NN12" t="inlineStr"/>
+      <c r="NN12" s="108" t="inlineStr"/>
       <c r="NO12" s="108" t="inlineStr"/>
       <c r="NP12" s="108" t="inlineStr"/>
     </row>
@@ -9022,7 +9022,7 @@
           <t>15.38%</t>
         </is>
       </c>
-      <c r="NN13" t="inlineStr">
+      <c r="NN13" s="108" t="inlineStr">
         <is>
           <t>46.15%</t>
         </is>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="NP13" s="108" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>88.46%</t>
         </is>
       </c>
     </row>
@@ -9138,7 +9138,7 @@
         <v>0</v>
       </c>
       <c r="NJ14" s="108" t="inlineStr"/>
-      <c r="NN14" t="inlineStr"/>
+      <c r="NN14" s="108" t="inlineStr"/>
       <c r="NO14" s="108" t="inlineStr"/>
       <c r="NP14" s="108" t="inlineStr"/>
     </row>
@@ -9692,7 +9692,7 @@
       <c r="NC15" s="208" t="n"/>
       <c r="ND15" s="208" t="n"/>
       <c r="NJ15" s="108" t="inlineStr"/>
-      <c r="NN15" t="inlineStr"/>
+      <c r="NN15" s="108" t="inlineStr"/>
       <c r="NO15" s="108" t="inlineStr"/>
       <c r="NP15" s="108" t="inlineStr"/>
     </row>
@@ -9799,7 +9799,7 @@
         <v>1735.5</v>
       </c>
       <c r="NJ16" s="108" t="inlineStr"/>
-      <c r="NN16" t="inlineStr"/>
+      <c r="NN16" s="108" t="inlineStr"/>
       <c r="NO16" s="108" t="inlineStr"/>
       <c r="NP16" s="108" t="inlineStr"/>
     </row>
@@ -10065,7 +10065,7 @@
         <v>0</v>
       </c>
       <c r="NJ17" s="108" t="inlineStr"/>
-      <c r="NN17" t="inlineStr"/>
+      <c r="NN17" s="108" t="inlineStr"/>
       <c r="NO17" s="108" t="inlineStr"/>
       <c r="NP17" s="108" t="inlineStr"/>
     </row>
@@ -10331,7 +10331,7 @@
         <v>5</v>
       </c>
       <c r="NJ18" s="108" t="inlineStr"/>
-      <c r="NN18" t="inlineStr"/>
+      <c r="NN18" s="108" t="inlineStr"/>
       <c r="NO18" s="108" t="inlineStr"/>
       <c r="NP18" s="108" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Cleaned things up a bit and squashed a few bugs.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -3053,9 +3053,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="H19:Q19"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="H19:Q19"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="NP2" s="108" t="inlineStr">
         <is>
-          <t>dsfg</t>
+          <t>4535</t>
         </is>
       </c>
     </row>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="NP13" s="108" t="inlineStr">
         <is>
-          <t>88.46%</t>
+          <t>76.92%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on making it remember the size and location of the window when moved.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -3269,7 +3269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:NP27"/>
+  <dimension ref="A1:NE27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="FH2" activePane="bottomRight" state="frozen"/>
@@ -4391,39 +4391,6 @@
         <v>45657</v>
       </c>
       <c r="NE1" s="240" t="n">
-        <v>45658</v>
-      </c>
-      <c r="NF1" s="240" t="n">
-        <v>45659</v>
-      </c>
-      <c r="NG1" s="240" t="n">
-        <v>45660</v>
-      </c>
-      <c r="NH1" s="240" t="n">
-        <v>45661</v>
-      </c>
-      <c r="NI1" s="240" t="n">
-        <v>45662</v>
-      </c>
-      <c r="NJ1" s="240" t="n">
-        <v>45663</v>
-      </c>
-      <c r="NK1" s="240" t="n">
-        <v>45664</v>
-      </c>
-      <c r="NL1" s="240" t="n">
-        <v>45665</v>
-      </c>
-      <c r="NM1" s="240" t="n">
-        <v>45666</v>
-      </c>
-      <c r="NN1" s="240" t="n">
-        <v>45667</v>
-      </c>
-      <c r="NO1" s="240" t="n">
-        <v>45668</v>
-      </c>
-      <c r="NP1" s="240" t="n">
         <v>45669</v>
       </c>
     </row>
@@ -4918,24 +4885,9 @@
       <c r="FX2" s="108" t="n">
         <v>60</v>
       </c>
-      <c r="NJ2" s="108" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
-      </c>
-      <c r="NN2" s="108" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="NO2" s="108" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="NP2" s="108" t="inlineStr">
-        <is>
-          <t>4535</t>
+      <c r="NE2" s="108" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -5206,10 +5158,7 @@
       <c r="FO3" s="108" t="n">
         <v>0</v>
       </c>
-      <c r="NJ3" s="108" t="inlineStr"/>
-      <c r="NN3" s="108" t="inlineStr"/>
-      <c r="NO3" s="108" t="inlineStr"/>
-      <c r="NP3" s="108" t="inlineStr"/>
+      <c r="NE3" s="108" t="inlineStr"/>
     </row>
     <row r="4" ht="15" customHeight="1" s="110">
       <c r="B4" s="204" t="inlineStr">
@@ -5472,10 +5421,7 @@
       <c r="FO4" s="108" t="n">
         <v>1</v>
       </c>
-      <c r="NJ4" s="108" t="inlineStr"/>
-      <c r="NN4" s="108" t="inlineStr"/>
-      <c r="NO4" s="108" t="inlineStr"/>
-      <c r="NP4" s="108" t="inlineStr"/>
+      <c r="NE4" s="108" t="inlineStr"/>
     </row>
     <row r="5" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B5" s="206" t="inlineStr">
@@ -5757,10 +5703,7 @@
       <c r="FO5" s="205" t="n">
         <v>4.03</v>
       </c>
-      <c r="NJ5" s="108" t="inlineStr"/>
-      <c r="NN5" s="108" t="inlineStr"/>
-      <c r="NO5" s="108" t="inlineStr"/>
-      <c r="NP5" s="108" t="inlineStr"/>
+      <c r="NE5" s="108" t="inlineStr"/>
     </row>
     <row r="6" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B6" s="206" t="inlineStr">
@@ -6033,10 +5976,7 @@
       <c r="FO6" s="205" t="n">
         <v>3.1</v>
       </c>
-      <c r="NJ6" s="108" t="inlineStr"/>
-      <c r="NN6" s="108" t="inlineStr"/>
-      <c r="NO6" s="108" t="inlineStr"/>
-      <c r="NP6" s="108" t="inlineStr"/>
+      <c r="NE6" s="108" t="inlineStr"/>
     </row>
     <row r="7" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="A7" s="208" t="n"/>
@@ -6343,10 +6283,7 @@
       <c r="FO7" s="207" t="n">
         <v>1</v>
       </c>
-      <c r="NJ7" s="108" t="inlineStr"/>
-      <c r="NN7" s="108" t="inlineStr"/>
-      <c r="NO7" s="108" t="inlineStr"/>
-      <c r="NP7" s="108" t="inlineStr"/>
+      <c r="NE7" s="108" t="inlineStr"/>
     </row>
     <row r="8" ht="15" customHeight="1" s="110">
       <c r="B8" s="210" t="inlineStr">
@@ -6624,10 +6561,7 @@
       <c r="FO8" s="207" t="n">
         <v>1</v>
       </c>
-      <c r="NJ8" s="108" t="inlineStr"/>
-      <c r="NN8" s="108" t="inlineStr"/>
-      <c r="NO8" s="108" t="inlineStr"/>
-      <c r="NP8" s="108" t="inlineStr"/>
+      <c r="NE8" s="108" t="inlineStr"/>
     </row>
     <row r="9" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="B9" s="211" t="inlineStr">
@@ -6731,10 +6665,7 @@
       <c r="FO9" s="207" t="n">
         <v>0</v>
       </c>
-      <c r="NJ9" s="108" t="inlineStr"/>
-      <c r="NN9" s="108" t="inlineStr"/>
-      <c r="NO9" s="108" t="inlineStr"/>
-      <c r="NP9" s="108" t="inlineStr"/>
+      <c r="NE9" s="108" t="inlineStr"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="110">
       <c r="A10" s="208" t="n"/>
@@ -7375,10 +7306,7 @@
       <c r="NB10" s="208" t="n"/>
       <c r="NC10" s="208" t="n"/>
       <c r="ND10" s="208" t="n"/>
-      <c r="NJ10" s="108" t="inlineStr"/>
-      <c r="NN10" s="108" t="inlineStr"/>
-      <c r="NO10" s="108" t="inlineStr"/>
-      <c r="NP10" s="108" t="inlineStr"/>
+      <c r="NE10" s="108" t="inlineStr"/>
     </row>
     <row r="11" ht="15" customHeight="1" s="110">
       <c r="A11" s="208" t="n"/>
@@ -7895,10 +7823,7 @@
       <c r="NB11" s="208" t="n"/>
       <c r="NC11" s="208" t="n"/>
       <c r="ND11" s="208" t="n"/>
-      <c r="NJ11" s="108" t="inlineStr"/>
-      <c r="NN11" s="108" t="inlineStr"/>
-      <c r="NO11" s="108" t="inlineStr"/>
-      <c r="NP11" s="108" t="inlineStr"/>
+      <c r="NE11" s="108" t="inlineStr"/>
     </row>
     <row r="12" ht="15" customHeight="1" s="110">
       <c r="A12" s="207" t="n"/>
@@ -8447,10 +8372,7 @@
       <c r="NB12" s="207" t="n"/>
       <c r="NC12" s="207" t="n"/>
       <c r="ND12" s="207" t="n"/>
-      <c r="NJ12" s="108" t="inlineStr"/>
-      <c r="NN12" s="108" t="inlineStr"/>
-      <c r="NO12" s="108" t="inlineStr"/>
-      <c r="NP12" s="108" t="inlineStr"/>
+      <c r="NE12" s="108" t="inlineStr"/>
     </row>
     <row r="13" ht="15" customHeight="1" s="110">
       <c r="A13" s="208" t="n"/>
@@ -9017,24 +8939,9 @@
       <c r="NB13" s="208" t="n"/>
       <c r="NC13" s="208" t="n"/>
       <c r="ND13" s="208" t="n"/>
-      <c r="NJ13" s="108" t="inlineStr">
-        <is>
-          <t>15.38%</t>
-        </is>
-      </c>
-      <c r="NN13" s="108" t="inlineStr">
-        <is>
-          <t>46.15%</t>
-        </is>
-      </c>
-      <c r="NO13" s="108" t="inlineStr">
-        <is>
-          <t>3.85%</t>
-        </is>
-      </c>
-      <c r="NP13" s="108" t="inlineStr">
-        <is>
-          <t>76.92%</t>
+      <c r="NE13" s="108" t="inlineStr">
+        <is>
+          <t>19.23%</t>
         </is>
       </c>
     </row>
@@ -9137,10 +9044,7 @@
       <c r="FO14" s="207" t="n">
         <v>0</v>
       </c>
-      <c r="NJ14" s="108" t="inlineStr"/>
-      <c r="NN14" s="108" t="inlineStr"/>
-      <c r="NO14" s="108" t="inlineStr"/>
-      <c r="NP14" s="108" t="inlineStr"/>
+      <c r="NE14" s="108" t="inlineStr"/>
     </row>
     <row r="15" ht="15" customHeight="1" s="110">
       <c r="A15" s="208" t="n"/>
@@ -9691,10 +9595,7 @@
       <c r="NB15" s="208" t="n"/>
       <c r="NC15" s="208" t="n"/>
       <c r="ND15" s="208" t="n"/>
-      <c r="NJ15" s="108" t="inlineStr"/>
-      <c r="NN15" s="108" t="inlineStr"/>
-      <c r="NO15" s="108" t="inlineStr"/>
-      <c r="NP15" s="108" t="inlineStr"/>
+      <c r="NE15" s="108" t="inlineStr"/>
     </row>
     <row r="16" ht="15" customHeight="1" s="110">
       <c r="B16" s="215" t="inlineStr">
@@ -9798,10 +9699,7 @@
       <c r="FO16" s="216" t="n">
         <v>1735.5</v>
       </c>
-      <c r="NJ16" s="108" t="inlineStr"/>
-      <c r="NN16" s="108" t="inlineStr"/>
-      <c r="NO16" s="108" t="inlineStr"/>
-      <c r="NP16" s="108" t="inlineStr"/>
+      <c r="NE16" s="108" t="inlineStr"/>
     </row>
     <row r="17" ht="15" customHeight="1" s="110">
       <c r="B17" s="215" t="inlineStr">
@@ -10064,10 +9962,7 @@
       <c r="FO17" s="108" t="n">
         <v>0</v>
       </c>
-      <c r="NJ17" s="108" t="inlineStr"/>
-      <c r="NN17" s="108" t="inlineStr"/>
-      <c r="NO17" s="108" t="inlineStr"/>
-      <c r="NP17" s="108" t="inlineStr"/>
+      <c r="NE17" s="108" t="inlineStr"/>
     </row>
     <row r="18" ht="15" customHeight="1" s="110">
       <c r="B18" s="215" t="inlineStr">
@@ -10330,10 +10225,7 @@
       <c r="FO18" s="108" t="n">
         <v>5</v>
       </c>
-      <c r="NJ18" s="108" t="inlineStr"/>
-      <c r="NN18" s="108" t="inlineStr"/>
-      <c r="NO18" s="108" t="inlineStr"/>
-      <c r="NP18" s="108" t="inlineStr"/>
+      <c r="NE18" s="108" t="inlineStr"/>
     </row>
     <row r="19" ht="15" customHeight="1" s="110">
       <c r="B19" s="108" t="inlineStr">

</xml_diff>

<commit_message>
Starting to implement date things (currently in a launchable state)
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -2010,7 +2010,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="2.71" customWidth="1" style="108" min="1" max="1"/>
     <col width="15.14" customWidth="1" style="108" min="2" max="2"/>
@@ -3053,9 +3053,9 @@
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D35:Q35"/>
     <mergeCell ref="H19:Q19"/>
-    <mergeCell ref="D35:Q35"/>
-    <mergeCell ref="F5:H5"/>
     <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K28:Q28"/>
@@ -3279,7 +3279,7 @@
       <selection pane="bottomRight" activeCell="FM10" activeCellId="0" sqref="FM10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="108" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="108" min="135" max="139"/>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="NE2" s="108" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>814</t>
         </is>
       </c>
     </row>
@@ -8941,7 +8941,7 @@
       <c r="ND13" s="208" t="n"/>
       <c r="NE13" s="108" t="inlineStr">
         <is>
-          <t>19.23%</t>
+          <t>76.92%</t>
         </is>
       </c>
     </row>
@@ -10303,7 +10303,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="108" min="1" max="1"/>
     <col width="17" customWidth="1" style="108" min="2" max="2"/>
@@ -10444,7 +10444,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="219" min="1" max="1"/>
     <col width="11" customWidth="1" style="219" min="2" max="2"/>
@@ -10657,7 +10657,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.85" customWidth="1" style="225" min="2" max="2"/>
     <col width="12" customWidth="1" style="225" min="3" max="3"/>
@@ -12358,7 +12358,7 @@
       <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="12.57" customWidth="1" style="225" min="1" max="4"/>
     <col width="10.14" customWidth="1" style="225" min="5" max="5"/>

</xml_diff>

<commit_message>
Addingthe ability to auto load the most recent workbook.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -25,13 +25,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="d\-mmm"/>
     <numFmt numFmtId="167" formatCode="d\-mmm\-yy"/>
     <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="169" formatCode="DD-MMM"/>
+    <numFmt numFmtId="170" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -3269,7 +3270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:PO27"/>
+  <dimension ref="A1:PP27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="FH2" activePane="bottomRight" state="frozen"/>
@@ -3289,69 +3290,6 @@
     <col width="10.57" customWidth="1" style="108" min="164" max="165"/>
     <col width="10.57" customWidth="1" style="108" min="167" max="167"/>
     <col width="10.57" customWidth="1" style="108" min="171" max="171"/>
-    <col width="12" customWidth="1" style="110" min="369" max="369"/>
-    <col width="12" customWidth="1" style="110" min="370" max="370"/>
-    <col width="12" customWidth="1" style="110" min="371" max="371"/>
-    <col width="12" customWidth="1" style="110" min="372" max="372"/>
-    <col width="12" customWidth="1" style="110" min="373" max="373"/>
-    <col width="12" customWidth="1" style="110" min="374" max="374"/>
-    <col width="12" customWidth="1" style="110" min="375" max="375"/>
-    <col width="12" customWidth="1" style="110" min="376" max="376"/>
-    <col width="12" customWidth="1" style="110" min="377" max="377"/>
-    <col width="12" customWidth="1" style="110" min="378" max="378"/>
-    <col width="12" customWidth="1" style="110" min="379" max="379"/>
-    <col width="12" customWidth="1" style="110" min="380" max="380"/>
-    <col width="12" customWidth="1" style="110" min="381" max="381"/>
-    <col width="12" customWidth="1" style="110" min="382" max="382"/>
-    <col width="12" customWidth="1" style="110" min="383" max="383"/>
-    <col width="12" customWidth="1" style="110" min="384" max="384"/>
-    <col width="12" customWidth="1" style="110" min="385" max="385"/>
-    <col width="12" customWidth="1" style="110" min="386" max="386"/>
-    <col width="12" customWidth="1" style="110" min="387" max="387"/>
-    <col width="12" customWidth="1" style="110" min="388" max="388"/>
-    <col width="12" customWidth="1" style="110" min="389" max="389"/>
-    <col width="12" customWidth="1" style="110" min="390" max="390"/>
-    <col width="12" customWidth="1" style="110" min="391" max="391"/>
-    <col width="12" customWidth="1" style="110" min="392" max="392"/>
-    <col width="12" customWidth="1" style="110" min="393" max="393"/>
-    <col width="12" customWidth="1" style="110" min="394" max="394"/>
-    <col width="12" customWidth="1" style="110" min="395" max="395"/>
-    <col width="12" customWidth="1" style="110" min="396" max="396"/>
-    <col width="12" customWidth="1" style="110" min="397" max="397"/>
-    <col width="12" customWidth="1" style="110" min="398" max="398"/>
-    <col width="12" customWidth="1" style="110" min="399" max="399"/>
-    <col width="12" customWidth="1" style="110" min="400" max="400"/>
-    <col width="12" customWidth="1" style="110" min="401" max="401"/>
-    <col width="12" customWidth="1" style="110" min="402" max="402"/>
-    <col width="12" customWidth="1" style="110" min="403" max="403"/>
-    <col width="12" customWidth="1" style="110" min="404" max="404"/>
-    <col width="12" customWidth="1" style="110" min="405" max="405"/>
-    <col width="12" customWidth="1" style="110" min="406" max="406"/>
-    <col width="12" customWidth="1" style="110" min="407" max="407"/>
-    <col width="12" customWidth="1" style="110" min="408" max="408"/>
-    <col width="12" customWidth="1" style="110" min="409" max="409"/>
-    <col width="12" customWidth="1" style="110" min="410" max="410"/>
-    <col width="12" customWidth="1" style="110" min="411" max="411"/>
-    <col width="12" customWidth="1" style="110" min="412" max="412"/>
-    <col width="12" customWidth="1" style="110" min="413" max="413"/>
-    <col width="12" customWidth="1" style="110" min="414" max="414"/>
-    <col width="12" customWidth="1" style="110" min="415" max="415"/>
-    <col width="12" customWidth="1" style="110" min="416" max="416"/>
-    <col width="12" customWidth="1" style="110" min="417" max="417"/>
-    <col width="12" customWidth="1" style="110" min="418" max="418"/>
-    <col width="12" customWidth="1" style="110" min="419" max="419"/>
-    <col width="12" customWidth="1" style="110" min="420" max="420"/>
-    <col width="12" customWidth="1" style="110" min="421" max="421"/>
-    <col width="12" customWidth="1" style="110" min="422" max="422"/>
-    <col width="12" customWidth="1" style="110" min="423" max="423"/>
-    <col width="12" customWidth="1" style="110" min="424" max="424"/>
-    <col width="12" customWidth="1" style="110" min="425" max="425"/>
-    <col width="12" customWidth="1" style="110" min="426" max="426"/>
-    <col width="12" customWidth="1" style="110" min="427" max="427"/>
-    <col width="12" customWidth="1" style="110" min="428" max="428"/>
-    <col width="12" customWidth="1" style="110" min="429" max="429"/>
-    <col width="12" customWidth="1" style="110" min="430" max="430"/>
-    <col width="12" customWidth="1" style="110" min="431" max="431"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="110">
@@ -4642,6 +4580,9 @@
       <c r="PO1" s="240" t="n">
         <v>45720</v>
       </c>
+      <c r="PP1" s="240" t="n">
+        <v>45721</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="110">
       <c r="B2" s="204" t="inlineStr">
@@ -5135,6 +5076,11 @@
       <c r="FX2" s="108" t="n">
         <v>60</v>
       </c>
+      <c r="PO2" s="108" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="110">
       <c r="B3" s="204" t="inlineStr">
@@ -5237,7 +5183,7 @@
       </c>
       <c r="BN3" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BT3" s="108" t="n">
@@ -5408,6 +5354,11 @@
       <c r="FO3" s="108" t="n">
         <v>0</v>
       </c>
+      <c r="PO3" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="110">
       <c r="B4" s="204" t="inlineStr">
@@ -5504,7 +5455,7 @@
       </c>
       <c r="BN4" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BT4" s="108" t="n">
@@ -5675,6 +5626,11 @@
       <c r="FO4" s="108" t="n">
         <v>1</v>
       </c>
+      <c r="PO4" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B5" s="206" t="inlineStr">
@@ -5777,7 +5733,7 @@
       </c>
       <c r="BN5" s="108" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BT5" s="205" t="n">
@@ -5961,6 +5917,11 @@
       <c r="FO5" s="205" t="n">
         <v>4.03</v>
       </c>
+      <c r="PO5" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B6" s="206" t="inlineStr">
@@ -6054,7 +6015,7 @@
       </c>
       <c r="BN6" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BT6" s="205" t="n">
@@ -6237,6 +6198,11 @@
       </c>
       <c r="FO6" s="205" t="n">
         <v>3.1</v>
+      </c>
+      <c r="PO6" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
     </row>
     <row r="7" ht="15" customFormat="1" customHeight="1" s="207">
@@ -6373,7 +6339,7 @@
       </c>
       <c r="BN7" s="208" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BO7" s="208" t="n"/>
@@ -6546,6 +6512,11 @@
       <c r="FO7" s="207" t="n">
         <v>1</v>
       </c>
+      <c r="PO7" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="110">
       <c r="B8" s="210" t="inlineStr">
@@ -6657,7 +6628,7 @@
       </c>
       <c r="BN8" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BT8" s="108" t="n">
@@ -6825,6 +6796,11 @@
       <c r="FO8" s="207" t="n">
         <v>1</v>
       </c>
+      <c r="PO8" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="B9" s="211" t="inlineStr">
@@ -6834,7 +6810,7 @@
       </c>
       <c r="BN9" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="DC9" s="207" t="n">
@@ -6932,6 +6908,11 @@
       </c>
       <c r="FO9" s="207" t="n">
         <v>0</v>
+      </c>
+      <c r="PO9" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="110">
@@ -7052,7 +7033,7 @@
       </c>
       <c r="BN10" s="208" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BO10" s="208" t="n"/>
@@ -7577,6 +7558,11 @@
       <c r="NB10" s="208" t="n"/>
       <c r="NC10" s="208" t="n"/>
       <c r="ND10" s="208" t="n"/>
+      <c r="PO10" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="110">
       <c r="A11" s="208" t="n"/>
@@ -7692,7 +7678,7 @@
       </c>
       <c r="BN11" s="208" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BO11" s="208" t="n"/>
@@ -8097,6 +8083,11 @@
       <c r="NB11" s="208" t="n"/>
       <c r="NC11" s="208" t="n"/>
       <c r="ND11" s="208" t="n"/>
+      <c r="PO11" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="110">
       <c r="A12" s="207" t="n"/>
@@ -8228,7 +8219,7 @@
       </c>
       <c r="BN12" s="207" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BO12" s="207" t="n"/>
@@ -8649,6 +8640,11 @@
       <c r="NB12" s="207" t="n"/>
       <c r="NC12" s="207" t="n"/>
       <c r="ND12" s="207" t="n"/>
+      <c r="PO12" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="110">
       <c r="A13" s="208" t="n"/>
@@ -8786,7 +8782,7 @@
       </c>
       <c r="BN13" s="208" t="inlineStr">
         <is>
-          <t>19.23%</t>
+          <t>76.92%</t>
         </is>
       </c>
       <c r="BO13" s="208" t="n"/>
@@ -9219,6 +9215,11 @@
       <c r="NB13" s="208" t="n"/>
       <c r="NC13" s="208" t="n"/>
       <c r="ND13" s="208" t="n"/>
+      <c r="PO13" s="108" t="inlineStr">
+        <is>
+          <t>61.54%</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="110">
       <c r="B14" s="213" t="inlineStr">
@@ -9228,7 +9229,7 @@
       </c>
       <c r="BN14" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="DD14" s="207" t="n">
@@ -9323,6 +9324,11 @@
       </c>
       <c r="FO14" s="207" t="n">
         <v>0</v>
+      </c>
+      <c r="PO14" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="110">
@@ -9463,7 +9469,7 @@
       </c>
       <c r="BN15" s="208" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BO15" s="208" t="n"/>
@@ -9876,6 +9882,11 @@
       <c r="NB15" s="208" t="n"/>
       <c r="NC15" s="208" t="n"/>
       <c r="ND15" s="208" t="n"/>
+      <c r="PO15" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="110">
       <c r="B16" s="215" t="inlineStr">
@@ -9885,7 +9896,7 @@
       </c>
       <c r="BN16" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="DC16" s="216" t="n">
@@ -9984,6 +9995,11 @@
       <c r="FO16" s="216" t="n">
         <v>1735.5</v>
       </c>
+      <c r="PO16" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="110">
       <c r="B17" s="215" t="inlineStr">
@@ -10086,7 +10102,7 @@
       </c>
       <c r="BN17" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BT17" s="207" t="n">
@@ -10251,6 +10267,11 @@
       <c r="FO17" s="108" t="n">
         <v>0</v>
       </c>
+      <c r="PO17" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="110">
       <c r="B18" s="215" t="inlineStr">
@@ -10353,7 +10374,7 @@
       </c>
       <c r="BN18" s="108" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>20</t>
         </is>
       </c>
       <c r="BT18" s="207" t="n">
@@ -10517,6 +10538,11 @@
       </c>
       <c r="FO18" s="108" t="n">
         <v>5</v>
+      </c>
+      <c r="PO18" s="108" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="110">

</xml_diff>

<commit_message>
Got the info to add in the correct place in the excel document.
</commit_message>
<xml_diff>
--- a/myenv/Excel_UI/Boxing Tier.xlsx
+++ b/myenv/Excel_UI/Boxing Tier.xlsx
@@ -3269,7 +3269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:QL27"/>
+  <dimension ref="A1:SH27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="FH2" activePane="bottomRight" state="frozen"/>
@@ -4648,6 +4648,150 @@
       <c r="QL1" s="240" t="n">
         <v>45743</v>
       </c>
+      <c r="QM1" s="240" t="n">
+        <v>45744</v>
+      </c>
+      <c r="QN1" s="240" t="n">
+        <v>45745</v>
+      </c>
+      <c r="QO1" s="240" t="n">
+        <v>45746</v>
+      </c>
+      <c r="QP1" s="240" t="n">
+        <v>45747</v>
+      </c>
+      <c r="QQ1" s="240" t="n">
+        <v>45748</v>
+      </c>
+      <c r="QR1" s="240" t="n">
+        <v>45749</v>
+      </c>
+      <c r="QS1" s="240" t="n">
+        <v>45750</v>
+      </c>
+      <c r="QT1" s="240" t="n">
+        <v>45751</v>
+      </c>
+      <c r="QU1" s="240" t="n">
+        <v>45752</v>
+      </c>
+      <c r="QV1" s="240" t="n">
+        <v>45753</v>
+      </c>
+      <c r="QW1" s="240" t="n">
+        <v>45754</v>
+      </c>
+      <c r="QX1" s="240" t="n">
+        <v>45755</v>
+      </c>
+      <c r="QY1" s="240" t="n">
+        <v>45756</v>
+      </c>
+      <c r="QZ1" s="240" t="n">
+        <v>45757</v>
+      </c>
+      <c r="RA1" s="240" t="n">
+        <v>45758</v>
+      </c>
+      <c r="RB1" s="240" t="n">
+        <v>45759</v>
+      </c>
+      <c r="RC1" s="240" t="n">
+        <v>45760</v>
+      </c>
+      <c r="RD1" s="240" t="n">
+        <v>45761</v>
+      </c>
+      <c r="RE1" s="240" t="n">
+        <v>45762</v>
+      </c>
+      <c r="RF1" s="240" t="n">
+        <v>45763</v>
+      </c>
+      <c r="RG1" s="240" t="n">
+        <v>45764</v>
+      </c>
+      <c r="RH1" s="240" t="n">
+        <v>45765</v>
+      </c>
+      <c r="RI1" s="240" t="n">
+        <v>45766</v>
+      </c>
+      <c r="RJ1" s="240" t="n">
+        <v>45767</v>
+      </c>
+      <c r="RK1" s="240" t="n">
+        <v>45768</v>
+      </c>
+      <c r="RL1" s="240" t="n">
+        <v>45769</v>
+      </c>
+      <c r="RM1" s="240" t="n">
+        <v>45770</v>
+      </c>
+      <c r="RN1" s="240" t="n">
+        <v>45771</v>
+      </c>
+      <c r="RO1" s="240" t="n">
+        <v>45772</v>
+      </c>
+      <c r="RP1" s="240" t="n">
+        <v>45773</v>
+      </c>
+      <c r="RQ1" s="240" t="n">
+        <v>45774</v>
+      </c>
+      <c r="RR1" s="240" t="n">
+        <v>45775</v>
+      </c>
+      <c r="RS1" s="240" t="n">
+        <v>45776</v>
+      </c>
+      <c r="RT1" s="240" t="n">
+        <v>45777</v>
+      </c>
+      <c r="RU1" s="240" t="n">
+        <v>45778</v>
+      </c>
+      <c r="RV1" s="240" t="n">
+        <v>45779</v>
+      </c>
+      <c r="RW1" s="240" t="n">
+        <v>45780</v>
+      </c>
+      <c r="RX1" s="240" t="n">
+        <v>45781</v>
+      </c>
+      <c r="RY1" s="240" t="n">
+        <v>45782</v>
+      </c>
+      <c r="RZ1" s="240" t="n">
+        <v>45783</v>
+      </c>
+      <c r="SA1" s="240" t="n">
+        <v>45784</v>
+      </c>
+      <c r="SB1" s="240" t="n">
+        <v>45785</v>
+      </c>
+      <c r="SC1" s="240" t="n">
+        <v>45786</v>
+      </c>
+      <c r="SD1" s="240" t="n">
+        <v>45787</v>
+      </c>
+      <c r="SE1" s="240" t="n">
+        <v>45788</v>
+      </c>
+      <c r="SF1" s="240" t="n">
+        <v>45789</v>
+      </c>
+      <c r="SG1" s="240" t="n">
+        <v>45790</v>
+      </c>
+      <c r="SH1" s="240" t="n">
+        <v>45791</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="110">
       <c r="B2" s="204" t="inlineStr">
@@ -5140,6 +5284,11 @@
       <c r="FX2" s="108" t="n">
         <v>60</v>
       </c>
+      <c r="SH2" s="108" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="110">
       <c r="B3" s="204" t="inlineStr">
@@ -5408,6 +5557,11 @@
       <c r="FO3" s="108" t="n">
         <v>0</v>
       </c>
+      <c r="SH3" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="110">
       <c r="B4" s="204" t="inlineStr">
@@ -5670,6 +5824,11 @@
       <c r="FO4" s="108" t="n">
         <v>1</v>
       </c>
+      <c r="SH4" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B5" s="206" t="inlineStr">
@@ -5951,6 +6110,11 @@
       <c r="FO5" s="205" t="n">
         <v>4.03</v>
       </c>
+      <c r="SH5" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15" customFormat="1" customHeight="1" s="205">
       <c r="B6" s="206" t="inlineStr">
@@ -6222,6 +6386,11 @@
       </c>
       <c r="FO6" s="205" t="n">
         <v>3.1</v>
+      </c>
+      <c r="SH6" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="7" ht="15" customFormat="1" customHeight="1" s="207">
@@ -6529,6 +6698,11 @@
       <c r="FO7" s="207" t="n">
         <v>1</v>
       </c>
+      <c r="SH7" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="110">
       <c r="B8" s="210" t="inlineStr">
@@ -6806,6 +6980,11 @@
       <c r="FO8" s="207" t="n">
         <v>1</v>
       </c>
+      <c r="SH8" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="15" customFormat="1" customHeight="1" s="207">
       <c r="B9" s="211" t="inlineStr">
@@ -6908,6 +7087,11 @@
       </c>
       <c r="FO9" s="207" t="n">
         <v>0</v>
+      </c>
+      <c r="SH9" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="110">
@@ -7549,6 +7733,11 @@
       <c r="NB10" s="208" t="n"/>
       <c r="NC10" s="208" t="n"/>
       <c r="ND10" s="208" t="n"/>
+      <c r="SH10" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="110">
       <c r="A11" s="208" t="n"/>
@@ -8065,6 +8254,11 @@
       <c r="NB11" s="208" t="n"/>
       <c r="NC11" s="208" t="n"/>
       <c r="ND11" s="208" t="n"/>
+      <c r="SH11" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="110">
       <c r="A12" s="207" t="n"/>
@@ -8613,6 +8807,11 @@
       <c r="NB12" s="207" t="n"/>
       <c r="NC12" s="207" t="n"/>
       <c r="ND12" s="207" t="n"/>
+      <c r="SH12" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="110">
       <c r="A13" s="208" t="n"/>
@@ -9179,6 +9378,11 @@
       <c r="NB13" s="208" t="n"/>
       <c r="NC13" s="208" t="n"/>
       <c r="ND13" s="208" t="n"/>
+      <c r="SH13" s="108" t="inlineStr">
+        <is>
+          <t>23.08%</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="110">
       <c r="B14" s="213" t="inlineStr">
@@ -9278,6 +9482,11 @@
       </c>
       <c r="FO14" s="207" t="n">
         <v>0</v>
+      </c>
+      <c r="SH14" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="110">
@@ -9829,6 +10038,11 @@
       <c r="NB15" s="208" t="n"/>
       <c r="NC15" s="208" t="n"/>
       <c r="ND15" s="208" t="n"/>
+      <c r="SH15" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="110">
       <c r="B16" s="215" t="inlineStr">
@@ -9932,6 +10146,11 @@
       <c r="FO16" s="216" t="n">
         <v>1735.5</v>
       </c>
+      <c r="SH16" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="110">
       <c r="B17" s="215" t="inlineStr">
@@ -10194,6 +10413,11 @@
       <c r="FO17" s="108" t="n">
         <v>0</v>
       </c>
+      <c r="SH17" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="110">
       <c r="B18" s="215" t="inlineStr">
@@ -10455,6 +10679,11 @@
       </c>
       <c r="FO18" s="108" t="n">
         <v>5</v>
+      </c>
+      <c r="SH18" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="110">

</xml_diff>